<commit_message>
enter -99 for missing UTM coor (mostly in trench/truck sites, and remove empty at M25 on 2/25/17
</commit_message>
<xml_diff>
--- a/Pit_Output/2017-02-24/PIT_MTR4_2000/pit_20170224_MTR4_2000.xlsx
+++ b/Pit_Output/2017-02-24/PIT_MTR4_2000/pit_20170224_MTR4_2000.xlsx
@@ -1,17 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hpm/D_DRIVE/GeoHackWeek/snowex/Pit_Output/2017-02-24/PIT_MTR4_2000/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="16380" windowHeight="8200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="PIT" sheetId="1" r:id="rId1"/>
     <sheet name="METADATA" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -594,7 +605,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
+        <charset val="134"/>
       </rPr>
       <t>Precipitation</t>
     </r>
@@ -632,7 +643,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
+        <charset val="134"/>
       </rPr>
       <t>Sky</t>
     </r>
@@ -664,7 +675,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
+        <charset val="134"/>
       </rPr>
       <t>Wind</t>
     </r>
@@ -708,7 +719,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
+        <charset val="134"/>
       </rPr>
       <t>Ground Condition</t>
     </r>
@@ -740,7 +751,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
+        <charset val="134"/>
       </rPr>
       <t>Soil Moisture</t>
     </r>
@@ -772,7 +783,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
+        <charset val="134"/>
       </rPr>
       <t>Ground Roughness</t>
     </r>
@@ -804,7 +815,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
+        <charset val="134"/>
       </rPr>
       <t>Ground Vegetation</t>
     </r>
@@ -842,7 +853,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
+        <charset val="134"/>
       </rPr>
       <t>Height of Ground Vegetation</t>
     </r>
@@ -1024,7 +1035,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1826,265 +1837,326 @@
   </cellStyleXfs>
   <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2095,75 +2167,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2291,12 +2302,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -2326,12 +2337,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -2535,1646 +2546,1521 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AMK33"/>
+  <dimension ref="A1:AA33"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R22" sqref="R22:Z23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5:J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="30" hidden="1"/>
-    <col min="2" max="2" width="6.140625" style="31" customWidth="1"/>
-    <col min="3" max="3" width="1.140625" style="32" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" style="30" customWidth="1"/>
-    <col min="5" max="6" width="8.5703125" style="30" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="30" customWidth="1"/>
-    <col min="8" max="8" width="3.85546875" style="30" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="30" customWidth="1"/>
-    <col min="10" max="10" width="1.140625" style="30" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="30" customWidth="1"/>
-    <col min="12" max="15" width="6.140625" style="30" customWidth="1"/>
-    <col min="16" max="17" width="3.5703125" style="30" customWidth="1"/>
-    <col min="18" max="18" width="9.7109375" style="30" customWidth="1"/>
-    <col min="19" max="19" width="6.140625" style="30" customWidth="1"/>
-    <col min="20" max="20" width="1.140625" style="30" customWidth="1"/>
-    <col min="21" max="21" width="6.140625" style="30" customWidth="1"/>
-    <col min="22" max="22" width="1.140625" style="30" customWidth="1"/>
-    <col min="23" max="23" width="3.5703125" style="30" customWidth="1"/>
-    <col min="24" max="24" width="1.140625" style="30" customWidth="1"/>
-    <col min="25" max="25" width="3.42578125" style="30" customWidth="1"/>
-    <col min="26" max="26" width="3.5703125" style="30" customWidth="1"/>
-    <col min="27" max="1025" width="8.28515625" style="30" customWidth="1"/>
+    <col min="1" max="1" width="11.5" style="1" hidden="1"/>
+    <col min="2" max="2" width="6.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="1.1640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="6.1640625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="8.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="3.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="1.1640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="7.1640625" style="1" customWidth="1"/>
+    <col min="12" max="15" width="6.1640625" style="1" customWidth="1"/>
+    <col min="16" max="17" width="3.5" style="1" customWidth="1"/>
+    <col min="18" max="18" width="9.6640625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="6.1640625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="1.1640625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="6.1640625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="1.1640625" style="1" customWidth="1"/>
+    <col min="23" max="23" width="3.5" style="1" customWidth="1"/>
+    <col min="24" max="24" width="1.1640625" style="1" customWidth="1"/>
+    <col min="25" max="26" width="3.5" style="1" customWidth="1"/>
+    <col min="27" max="27" width="8.33203125" style="1" customWidth="1"/>
+    <col min="28" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:27" ht="15.95" customHeight="1">
-      <c r="B1" s="14" t="s">
+    <row r="1" spans="2:27" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B1" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="13" t="s">
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="12" t="s">
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="11" t="s">
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
+      <c r="R1" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="11"/>
-      <c r="AA1" s="30" t="s">
+      <c r="S1" s="77"/>
+      <c r="T1" s="77"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="77"/>
+      <c r="W1" s="77"/>
+      <c r="X1" s="77"/>
+      <c r="Y1" s="77"/>
+      <c r="Z1" s="77"/>
+      <c r="AA1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="2:27" ht="24" customHeight="1">
-      <c r="B2" s="10" t="s">
+    <row r="2" spans="2:27" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B2" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="8" t="s">
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="79">
+        <v>-99</v>
+      </c>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+      <c r="L2" s="79"/>
+      <c r="M2" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="7" t="s">
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
-      <c r="W2" s="7"/>
-      <c r="X2" s="7"/>
-      <c r="Y2" s="7"/>
-      <c r="Z2" s="7"/>
-    </row>
-    <row r="3" spans="2:27" ht="15" customHeight="1">
-      <c r="B3" s="10" t="s">
+      <c r="S2" s="80"/>
+      <c r="T2" s="80"/>
+      <c r="U2" s="80"/>
+      <c r="V2" s="80"/>
+      <c r="W2" s="80"/>
+      <c r="X2" s="80"/>
+      <c r="Y2" s="80"/>
+      <c r="Z2" s="80"/>
+    </row>
+    <row r="3" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B3" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="9" t="s">
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
-      <c r="W3" s="7"/>
-      <c r="X3" s="7"/>
-      <c r="Y3" s="7"/>
-      <c r="Z3" s="7"/>
-    </row>
-    <row r="4" spans="2:27" ht="29.1" customHeight="1">
-      <c r="B4" s="10" t="s">
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="79"/>
+      <c r="L3" s="79"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="47"/>
+      <c r="P3" s="47"/>
+      <c r="Q3" s="47"/>
+      <c r="R3" s="80"/>
+      <c r="S3" s="80"/>
+      <c r="T3" s="80"/>
+      <c r="U3" s="80"/>
+      <c r="V3" s="80"/>
+      <c r="W3" s="80"/>
+      <c r="X3" s="80"/>
+      <c r="Y3" s="80"/>
+      <c r="Z3" s="80"/>
+    </row>
+    <row r="4" spans="2:27" ht="29" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B4" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7"/>
-      <c r="U4" s="7"/>
-      <c r="V4" s="7"/>
-      <c r="W4" s="7"/>
-      <c r="X4" s="7"/>
-      <c r="Y4" s="7"/>
-      <c r="Z4" s="7"/>
-    </row>
-    <row r="5" spans="2:27" ht="15" customHeight="1">
-      <c r="B5" s="6" t="s">
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="79">
+        <v>-99</v>
+      </c>
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="79"/>
+      <c r="L4" s="79"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="47"/>
+      <c r="P4" s="47"/>
+      <c r="Q4" s="47"/>
+      <c r="R4" s="80"/>
+      <c r="S4" s="80"/>
+      <c r="T4" s="80"/>
+      <c r="U4" s="80"/>
+      <c r="V4" s="80"/>
+      <c r="W4" s="80"/>
+      <c r="X4" s="80"/>
+      <c r="Y4" s="80"/>
+      <c r="Z4" s="80"/>
+    </row>
+    <row r="5" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B5" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="5" t="s">
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="4" t="s">
+      <c r="G5" s="82"/>
+      <c r="H5" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="34" t="s">
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
+      <c r="K5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="L5" s="34"/>
-      <c r="M5" s="4" t="s">
+      <c r="L5" s="5"/>
+      <c r="M5" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="N5" s="4"/>
-      <c r="O5" s="8" t="s">
+      <c r="N5" s="72"/>
+      <c r="O5" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
-      <c r="W5" s="7"/>
-      <c r="X5" s="7"/>
-      <c r="Y5" s="7"/>
-      <c r="Z5" s="7"/>
-    </row>
-    <row r="6" spans="2:27" ht="27" customHeight="1">
-      <c r="B6" s="3" t="s">
+      <c r="P5" s="47"/>
+      <c r="Q5" s="47"/>
+      <c r="R5" s="80"/>
+      <c r="S5" s="80"/>
+      <c r="T5" s="80"/>
+      <c r="U5" s="80"/>
+      <c r="V5" s="80"/>
+      <c r="W5" s="80"/>
+      <c r="X5" s="80"/>
+      <c r="Y5" s="80"/>
+      <c r="Z5" s="80"/>
+    </row>
+    <row r="6" spans="2:27" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B6" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="2" t="s">
+      <c r="C6" s="83"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="29" t="s">
+      <c r="G6" s="84"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="85"/>
+      <c r="J6" s="85"/>
+      <c r="K6" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29" t="s">
+      <c r="L6" s="86"/>
+      <c r="M6" s="86" t="s">
         <v>20</v>
       </c>
-      <c r="N6" s="29"/>
-      <c r="O6" s="28" t="s">
+      <c r="N6" s="86"/>
+      <c r="O6" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="P6" s="28"/>
-      <c r="Q6" s="28"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7"/>
-      <c r="U6" s="7"/>
-      <c r="V6" s="7"/>
-      <c r="W6" s="7"/>
-      <c r="X6" s="7"/>
-      <c r="Y6" s="7"/>
-      <c r="Z6" s="7"/>
-    </row>
-    <row r="7" spans="2:27" s="35" customFormat="1" ht="15" customHeight="1">
-      <c r="B7" s="27" t="s">
+      <c r="P6" s="87"/>
+      <c r="Q6" s="87"/>
+      <c r="R6" s="80"/>
+      <c r="S6" s="80"/>
+      <c r="T6" s="80"/>
+      <c r="U6" s="80"/>
+      <c r="V6" s="80"/>
+      <c r="W6" s="80"/>
+      <c r="X6" s="80"/>
+      <c r="Y6" s="80"/>
+      <c r="Z6" s="80"/>
+    </row>
+    <row r="7" spans="2:27" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B7" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="26" t="s">
+      <c r="C7" s="88"/>
+      <c r="D7" s="88"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="88"/>
+      <c r="G7" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="26"/>
-      <c r="I7" s="25" t="s">
+      <c r="H7" s="66"/>
+      <c r="I7" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25"/>
-      <c r="O7" s="25"/>
-      <c r="P7" s="25"/>
-      <c r="Q7" s="25"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7"/>
-      <c r="U7" s="7"/>
-      <c r="V7" s="7"/>
-      <c r="W7" s="7"/>
-      <c r="X7" s="7"/>
-      <c r="Y7" s="7"/>
-      <c r="Z7" s="7"/>
-    </row>
-    <row r="8" spans="2:27" ht="37.15" customHeight="1">
-      <c r="B8" s="24" t="s">
+      <c r="J7" s="67"/>
+      <c r="K7" s="67"/>
+      <c r="L7" s="67"/>
+      <c r="M7" s="67"/>
+      <c r="N7" s="67"/>
+      <c r="O7" s="67"/>
+      <c r="P7" s="67"/>
+      <c r="Q7" s="67"/>
+      <c r="R7" s="80"/>
+      <c r="S7" s="80"/>
+      <c r="T7" s="80"/>
+      <c r="U7" s="80"/>
+      <c r="V7" s="80"/>
+      <c r="W7" s="80"/>
+      <c r="X7" s="80"/>
+      <c r="Y7" s="80"/>
+      <c r="Z7" s="80"/>
+    </row>
+    <row r="8" spans="2:27" ht="37.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B8" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="36" t="s">
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="37" t="s">
+      <c r="F8" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="38" t="s">
+      <c r="G8" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="37" t="s">
+      <c r="H8" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="23" t="s">
+      <c r="I8" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="22" t="s">
+      <c r="J8" s="69"/>
+      <c r="K8" s="69"/>
+      <c r="L8" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22"/>
-      <c r="O8" s="21" t="s">
+      <c r="M8" s="70"/>
+      <c r="N8" s="70"/>
+      <c r="O8" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="P8" s="4" t="s">
+      <c r="P8" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="Q8" s="4" t="s">
+      <c r="Q8" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="R8" s="20" t="s">
+      <c r="R8" s="73" t="s">
         <v>34</v>
       </c>
-      <c r="S8" s="20"/>
-      <c r="T8" s="20"/>
-      <c r="U8" s="20"/>
-      <c r="V8" s="20"/>
-      <c r="W8" s="20"/>
-      <c r="X8" s="20"/>
-      <c r="Y8" s="20"/>
-      <c r="Z8" s="20"/>
-    </row>
-    <row r="9" spans="2:27" ht="22.5" customHeight="1">
-      <c r="B9" s="39" t="s">
+      <c r="S8" s="73"/>
+      <c r="T8" s="73"/>
+      <c r="U8" s="73"/>
+      <c r="V8" s="73"/>
+      <c r="W8" s="73"/>
+      <c r="X8" s="73"/>
+      <c r="Y8" s="73"/>
+      <c r="Z8" s="73"/>
+    </row>
+    <row r="9" spans="2:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B9" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="41" t="s">
+      <c r="C9" s="11"/>
+      <c r="D9" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="42" t="s">
+      <c r="E9" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="43" t="s">
+      <c r="F9" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="G9" s="44" t="s">
+      <c r="G9" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="H9" s="45" t="s">
+      <c r="H9" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="I9" s="46" t="s">
+      <c r="I9" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="J9" s="46"/>
-      <c r="K9" s="46" t="s">
+      <c r="J9" s="17"/>
+      <c r="K9" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="L9" s="47" t="s">
+      <c r="L9" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="M9" s="47" t="s">
+      <c r="M9" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="N9" s="47" t="s">
+      <c r="N9" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="O9" s="21"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="20"/>
-      <c r="S9" s="20"/>
-      <c r="T9" s="20"/>
-      <c r="U9" s="20"/>
-      <c r="V9" s="20"/>
-      <c r="W9" s="20"/>
-      <c r="X9" s="20"/>
-      <c r="Y9" s="20"/>
-      <c r="Z9" s="20"/>
-    </row>
-    <row r="10" spans="2:27" ht="19.899999999999999" customHeight="1">
-      <c r="B10" s="48" t="s">
+      <c r="O9" s="71"/>
+      <c r="P9" s="72"/>
+      <c r="Q9" s="72"/>
+      <c r="R9" s="73"/>
+      <c r="S9" s="73"/>
+      <c r="T9" s="73"/>
+      <c r="U9" s="73"/>
+      <c r="V9" s="73"/>
+      <c r="W9" s="73"/>
+      <c r="X9" s="73"/>
+      <c r="Y9" s="73"/>
+      <c r="Z9" s="73"/>
+    </row>
+    <row r="10" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B10" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="49" t="s">
+      <c r="C10" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="50" t="s">
+      <c r="D10" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="34" t="s">
+      <c r="E10" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="33" t="s">
+      <c r="F10" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G10" s="50" t="s">
+      <c r="G10" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="33" t="s">
+      <c r="H10" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="I10" s="19" t="s">
+      <c r="I10" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="J10" s="18" t="s">
+      <c r="J10" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="K10" s="19" t="s">
+      <c r="K10" s="64" t="s">
         <v>49</v>
       </c>
-      <c r="L10" s="17" t="s">
+      <c r="L10" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="M10" s="17" t="s">
+      <c r="M10" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="N10" s="17" t="s">
+      <c r="N10" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="O10" s="16" t="s">
+      <c r="O10" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="P10" s="16" t="s">
+      <c r="P10" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="Q10" s="16" t="s">
+      <c r="Q10" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="R10" s="15" t="s">
+      <c r="R10" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="S10" s="15"/>
-      <c r="T10" s="15"/>
-      <c r="U10" s="15"/>
-      <c r="V10" s="15"/>
-      <c r="W10" s="15"/>
-      <c r="X10" s="15"/>
-      <c r="Y10" s="15"/>
-      <c r="Z10" s="15"/>
-    </row>
-    <row r="11" spans="2:27" ht="19.899999999999999" customHeight="1">
-      <c r="B11" s="48" t="s">
+      <c r="S10" s="57"/>
+      <c r="T10" s="57"/>
+      <c r="U10" s="57"/>
+      <c r="V10" s="57"/>
+      <c r="W10" s="57"/>
+      <c r="X10" s="57"/>
+      <c r="Y10" s="57"/>
+      <c r="Z10" s="57"/>
+    </row>
+    <row r="11" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B11" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="49" t="s">
+      <c r="C11" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="50" t="s">
+      <c r="D11" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="34" t="s">
+      <c r="E11" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="33" t="s">
+      <c r="F11" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="G11" s="50" t="s">
+      <c r="G11" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="H11" s="33" t="s">
+      <c r="H11" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="I11" s="19"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="16"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
-      <c r="T11" s="15"/>
-      <c r="U11" s="15"/>
-      <c r="V11" s="15"/>
-      <c r="W11" s="15"/>
-      <c r="X11" s="15"/>
-      <c r="Y11" s="15"/>
-      <c r="Z11" s="15"/>
-    </row>
-    <row r="12" spans="2:27" ht="19.899999999999999" customHeight="1">
-      <c r="B12" s="48" t="s">
+      <c r="I11" s="64"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="64"/>
+      <c r="L11" s="56"/>
+      <c r="M11" s="56"/>
+      <c r="N11" s="56"/>
+      <c r="O11" s="65"/>
+      <c r="P11" s="65"/>
+      <c r="Q11" s="65"/>
+      <c r="R11" s="57"/>
+      <c r="S11" s="57"/>
+      <c r="T11" s="57"/>
+      <c r="U11" s="57"/>
+      <c r="V11" s="57"/>
+      <c r="W11" s="57"/>
+      <c r="X11" s="57"/>
+      <c r="Y11" s="57"/>
+      <c r="Z11" s="57"/>
+    </row>
+    <row r="12" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B12" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="49" t="s">
+      <c r="C12" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="50" t="s">
+      <c r="D12" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="E12" s="34" t="s">
+      <c r="E12" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="33" t="s">
+      <c r="F12" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="50" t="s">
+      <c r="G12" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="H12" s="33" t="s">
+      <c r="H12" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="I12" s="19" t="s">
+      <c r="I12" s="64" t="s">
         <v>49</v>
       </c>
-      <c r="J12" s="18" t="s">
+      <c r="J12" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="K12" s="19" t="s">
+      <c r="K12" s="64" t="s">
         <v>60</v>
       </c>
-      <c r="L12" s="17" t="s">
+      <c r="L12" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="M12" s="17" t="s">
+      <c r="M12" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="N12" s="17" t="s">
+      <c r="N12" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="O12" s="16" t="s">
+      <c r="O12" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="P12" s="16" t="s">
+      <c r="P12" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="Q12" s="16" t="s">
+      <c r="Q12" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="R12" s="15" t="s">
+      <c r="R12" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="S12" s="15"/>
-      <c r="T12" s="15"/>
-      <c r="U12" s="15"/>
-      <c r="V12" s="15"/>
-      <c r="W12" s="15"/>
-      <c r="X12" s="15"/>
-      <c r="Y12" s="15"/>
-      <c r="Z12" s="15"/>
-    </row>
-    <row r="13" spans="2:27" ht="19.899999999999999" customHeight="1">
-      <c r="B13" s="48" t="s">
+      <c r="S12" s="57"/>
+      <c r="T12" s="57"/>
+      <c r="U12" s="57"/>
+      <c r="V12" s="57"/>
+      <c r="W12" s="57"/>
+      <c r="X12" s="57"/>
+      <c r="Y12" s="57"/>
+      <c r="Z12" s="57"/>
+    </row>
+    <row r="13" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="49" t="s">
+      <c r="C13" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="50" t="s">
+      <c r="D13" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="E13" s="34" t="s">
+      <c r="E13" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="F13" s="33" t="s">
+      <c r="F13" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="G13" s="50" t="s">
+      <c r="G13" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="H13" s="33" t="s">
+      <c r="H13" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="I13" s="19"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="16"/>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="16"/>
-      <c r="R13" s="15"/>
-      <c r="S13" s="15"/>
-      <c r="T13" s="15"/>
-      <c r="U13" s="15"/>
-      <c r="V13" s="15"/>
-      <c r="W13" s="15"/>
-      <c r="X13" s="15"/>
-      <c r="Y13" s="15"/>
-      <c r="Z13" s="15"/>
-    </row>
-    <row r="14" spans="2:27" ht="19.899999999999999" customHeight="1">
-      <c r="B14" s="48" t="s">
+      <c r="I13" s="64"/>
+      <c r="J13" s="54"/>
+      <c r="K13" s="64"/>
+      <c r="L13" s="56"/>
+      <c r="M13" s="56"/>
+      <c r="N13" s="56"/>
+      <c r="O13" s="65"/>
+      <c r="P13" s="65"/>
+      <c r="Q13" s="65"/>
+      <c r="R13" s="57"/>
+      <c r="S13" s="57"/>
+      <c r="T13" s="57"/>
+      <c r="U13" s="57"/>
+      <c r="V13" s="57"/>
+      <c r="W13" s="57"/>
+      <c r="X13" s="57"/>
+      <c r="Y13" s="57"/>
+      <c r="Z13" s="57"/>
+    </row>
+    <row r="14" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B14" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="C14" s="49" t="s">
+      <c r="C14" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="50" t="s">
+      <c r="D14" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="E14" s="34" t="s">
+      <c r="E14" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="F14" s="33" t="s">
+      <c r="F14" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G14" s="50" t="s">
+      <c r="G14" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="H14" s="33" t="s">
+      <c r="H14" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="I14" s="19" t="s">
+      <c r="I14" s="64" t="s">
         <v>60</v>
       </c>
-      <c r="J14" s="18" t="s">
+      <c r="J14" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="K14" s="19" t="s">
+      <c r="K14" s="64" t="s">
         <v>65</v>
       </c>
-      <c r="L14" s="17" t="s">
+      <c r="L14" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="M14" s="17" t="s">
+      <c r="M14" s="56" t="s">
         <v>79</v>
       </c>
-      <c r="N14" s="17" t="s">
+      <c r="N14" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="O14" s="16" t="s">
+      <c r="O14" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="P14" s="16" t="s">
+      <c r="P14" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="Q14" s="16" t="s">
+      <c r="Q14" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="R14" s="15" t="s">
+      <c r="R14" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="S14" s="15"/>
-      <c r="T14" s="15"/>
-      <c r="U14" s="15"/>
-      <c r="V14" s="15"/>
-      <c r="W14" s="15"/>
-      <c r="X14" s="15"/>
-      <c r="Y14" s="15"/>
-      <c r="Z14" s="15"/>
-    </row>
-    <row r="15" spans="2:27" ht="19.899999999999999" customHeight="1">
-      <c r="B15" s="48" t="s">
+      <c r="S14" s="57"/>
+      <c r="T14" s="57"/>
+      <c r="U14" s="57"/>
+      <c r="V14" s="57"/>
+      <c r="W14" s="57"/>
+      <c r="X14" s="57"/>
+      <c r="Y14" s="57"/>
+      <c r="Z14" s="57"/>
+    </row>
+    <row r="15" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B15" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="C15" s="49" t="s">
+      <c r="C15" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="50" t="s">
+      <c r="D15" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="E15" s="34" t="s">
+      <c r="E15" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="F15" s="33" t="s">
+      <c r="F15" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="G15" s="50" t="s">
+      <c r="G15" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="H15" s="33" t="s">
+      <c r="H15" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="I15" s="19"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="16"/>
-      <c r="P15" s="16"/>
-      <c r="Q15" s="16"/>
-      <c r="R15" s="15"/>
-      <c r="S15" s="15"/>
-      <c r="T15" s="15"/>
-      <c r="U15" s="15"/>
-      <c r="V15" s="15"/>
-      <c r="W15" s="15"/>
-      <c r="X15" s="15"/>
-      <c r="Y15" s="15"/>
-      <c r="Z15" s="15"/>
-    </row>
-    <row r="16" spans="2:27" ht="19.899999999999999" customHeight="1">
-      <c r="B16" s="48" t="s">
+      <c r="I15" s="64"/>
+      <c r="J15" s="54"/>
+      <c r="K15" s="64"/>
+      <c r="L15" s="56"/>
+      <c r="M15" s="56"/>
+      <c r="N15" s="56"/>
+      <c r="O15" s="65"/>
+      <c r="P15" s="65"/>
+      <c r="Q15" s="65"/>
+      <c r="R15" s="57"/>
+      <c r="S15" s="57"/>
+      <c r="T15" s="57"/>
+      <c r="U15" s="57"/>
+      <c r="V15" s="57"/>
+      <c r="W15" s="57"/>
+      <c r="X15" s="57"/>
+      <c r="Y15" s="57"/>
+      <c r="Z15" s="57"/>
+    </row>
+    <row r="16" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="C16" s="49" t="s">
+      <c r="C16" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="50" t="s">
+      <c r="D16" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="E16" s="34" t="s">
+      <c r="E16" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="F16" s="33" t="s">
+      <c r="F16" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G16" s="50" t="s">
+      <c r="G16" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="H16" s="33" t="s">
+      <c r="H16" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="I16" s="19" t="s">
+      <c r="I16" s="64" t="s">
         <v>65</v>
       </c>
-      <c r="J16" s="18" t="s">
+      <c r="J16" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="K16" s="19" t="s">
+      <c r="K16" s="64" t="s">
         <v>91</v>
       </c>
-      <c r="L16" s="17" t="s">
+      <c r="L16" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="M16" s="17" t="s">
+      <c r="M16" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="N16" s="17" t="s">
+      <c r="N16" s="56" t="s">
         <v>79</v>
       </c>
-      <c r="O16" s="16" t="s">
+      <c r="O16" s="65" t="s">
         <v>93</v>
       </c>
-      <c r="P16" s="16" t="s">
+      <c r="P16" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="Q16" s="16" t="s">
+      <c r="Q16" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="R16" s="15" t="s">
+      <c r="R16" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="S16" s="15"/>
-      <c r="T16" s="15"/>
-      <c r="U16" s="15"/>
-      <c r="V16" s="15"/>
-      <c r="W16" s="15"/>
-      <c r="X16" s="15"/>
-      <c r="Y16" s="15"/>
-      <c r="Z16" s="15"/>
-    </row>
-    <row r="17" spans="2:26" ht="19.899999999999999" customHeight="1">
-      <c r="B17" s="48" t="s">
+      <c r="S16" s="57"/>
+      <c r="T16" s="57"/>
+      <c r="U16" s="57"/>
+      <c r="V16" s="57"/>
+      <c r="W16" s="57"/>
+      <c r="X16" s="57"/>
+      <c r="Y16" s="57"/>
+      <c r="Z16" s="57"/>
+    </row>
+    <row r="17" spans="2:26" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B17" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="C17" s="49" t="s">
+      <c r="C17" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="50" t="s">
+      <c r="D17" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="E17" s="34" t="s">
+      <c r="E17" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F17" s="33" t="s">
+      <c r="F17" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="G17" s="50" t="s">
+      <c r="G17" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="H17" s="33" t="s">
+      <c r="H17" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="I17" s="19"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="16"/>
-      <c r="P17" s="16"/>
-      <c r="Q17" s="16"/>
-      <c r="R17" s="15"/>
-      <c r="S17" s="15"/>
-      <c r="T17" s="15"/>
-      <c r="U17" s="15"/>
-      <c r="V17" s="15"/>
-      <c r="W17" s="15"/>
-      <c r="X17" s="15"/>
-      <c r="Y17" s="15"/>
-      <c r="Z17" s="15"/>
-    </row>
-    <row r="18" spans="2:26" ht="19.899999999999999" customHeight="1">
-      <c r="B18" s="48" t="s">
+      <c r="I17" s="64"/>
+      <c r="J17" s="54"/>
+      <c r="K17" s="64"/>
+      <c r="L17" s="56"/>
+      <c r="M17" s="56"/>
+      <c r="N17" s="56"/>
+      <c r="O17" s="65"/>
+      <c r="P17" s="65"/>
+      <c r="Q17" s="65"/>
+      <c r="R17" s="57"/>
+      <c r="S17" s="57"/>
+      <c r="T17" s="57"/>
+      <c r="U17" s="57"/>
+      <c r="V17" s="57"/>
+      <c r="W17" s="57"/>
+      <c r="X17" s="57"/>
+      <c r="Y17" s="57"/>
+      <c r="Z17" s="57"/>
+    </row>
+    <row r="18" spans="2:26" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="49" t="s">
+      <c r="C18" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="50" t="s">
+      <c r="D18" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="E18" s="34" t="s">
+      <c r="E18" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="F18" s="33" t="s">
+      <c r="F18" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="G18" s="50" t="s">
+      <c r="G18" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="H18" s="33" t="s">
+      <c r="H18" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="I18" s="19" t="s">
+      <c r="I18" s="64" t="s">
         <v>91</v>
       </c>
-      <c r="J18" s="18" t="s">
+      <c r="J18" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="K18" s="19" t="s">
+      <c r="K18" s="64" t="s">
         <v>105</v>
       </c>
-      <c r="L18" s="17" t="s">
+      <c r="L18" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="M18" s="17" t="s">
+      <c r="M18" s="56" t="s">
         <v>79</v>
       </c>
-      <c r="N18" s="17" t="s">
+      <c r="N18" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="O18" s="16" t="s">
+      <c r="O18" s="65" t="s">
         <v>93</v>
       </c>
-      <c r="P18" s="16" t="s">
+      <c r="P18" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="Q18" s="16" t="s">
+      <c r="Q18" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="R18" s="15" t="s">
+      <c r="R18" s="57" t="s">
         <v>106</v>
       </c>
-      <c r="S18" s="15"/>
-      <c r="T18" s="15"/>
-      <c r="U18" s="15"/>
-      <c r="V18" s="15"/>
-      <c r="W18" s="15"/>
-      <c r="X18" s="15"/>
-      <c r="Y18" s="15"/>
-      <c r="Z18" s="15"/>
-    </row>
-    <row r="19" spans="2:26" ht="19.899999999999999" customHeight="1">
-      <c r="B19" s="48" t="s">
+      <c r="S18" s="57"/>
+      <c r="T18" s="57"/>
+      <c r="U18" s="57"/>
+      <c r="V18" s="57"/>
+      <c r="W18" s="57"/>
+      <c r="X18" s="57"/>
+      <c r="Y18" s="57"/>
+      <c r="Z18" s="57"/>
+    </row>
+    <row r="19" spans="2:26" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="C19" s="49" t="s">
+      <c r="C19" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="50" t="s">
+      <c r="D19" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="E19" s="34" t="s">
+      <c r="E19" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="F19" s="33" t="s">
+      <c r="F19" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G19" s="50" t="s">
+      <c r="G19" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="H19" s="33" t="s">
+      <c r="H19" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="I19" s="19"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="17"/>
-      <c r="N19" s="17"/>
-      <c r="O19" s="16"/>
-      <c r="P19" s="16"/>
-      <c r="Q19" s="16"/>
-      <c r="R19" s="15"/>
-      <c r="S19" s="15"/>
-      <c r="T19" s="15"/>
-      <c r="U19" s="15"/>
-      <c r="V19" s="15"/>
-      <c r="W19" s="15"/>
-      <c r="X19" s="15"/>
-      <c r="Y19" s="15"/>
-      <c r="Z19" s="15"/>
-    </row>
-    <row r="20" spans="2:26" ht="19.899999999999999" customHeight="1">
-      <c r="B20" s="48" t="s">
+      <c r="I19" s="64"/>
+      <c r="J19" s="54"/>
+      <c r="K19" s="64"/>
+      <c r="L19" s="56"/>
+      <c r="M19" s="56"/>
+      <c r="N19" s="56"/>
+      <c r="O19" s="65"/>
+      <c r="P19" s="65"/>
+      <c r="Q19" s="65"/>
+      <c r="R19" s="57"/>
+      <c r="S19" s="57"/>
+      <c r="T19" s="57"/>
+      <c r="U19" s="57"/>
+      <c r="V19" s="57"/>
+      <c r="W19" s="57"/>
+      <c r="X19" s="57"/>
+      <c r="Y19" s="57"/>
+      <c r="Z19" s="57"/>
+    </row>
+    <row r="20" spans="2:26" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="C20" s="49" t="s">
+      <c r="C20" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="50" t="s">
+      <c r="D20" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="E20" s="34" t="s">
+      <c r="E20" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="F20" s="33" t="s">
+      <c r="F20" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="G20" s="50" t="s">
+      <c r="G20" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="H20" s="33" t="s">
+      <c r="H20" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="I20" s="19" t="s">
+      <c r="I20" s="64" t="s">
         <v>105</v>
       </c>
-      <c r="J20" s="18" t="s">
+      <c r="J20" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="K20" s="19" t="s">
+      <c r="K20" s="64" t="s">
         <v>117</v>
       </c>
-      <c r="L20" s="17" t="s">
+      <c r="L20" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="M20" s="17" t="s">
+      <c r="M20" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="N20" s="17" t="s">
+      <c r="N20" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="O20" s="16" t="s">
+      <c r="O20" s="65" t="s">
         <v>118</v>
       </c>
-      <c r="P20" s="16" t="s">
+      <c r="P20" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="Q20" s="16" t="s">
+      <c r="Q20" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="R20" s="15" t="s">
+      <c r="R20" s="57" t="s">
         <v>119</v>
       </c>
-      <c r="S20" s="15"/>
-      <c r="T20" s="15"/>
-      <c r="U20" s="15"/>
-      <c r="V20" s="15"/>
-      <c r="W20" s="15"/>
-      <c r="X20" s="15"/>
-      <c r="Y20" s="15"/>
-      <c r="Z20" s="15"/>
-    </row>
-    <row r="21" spans="2:26" ht="19.899999999999999" customHeight="1">
-      <c r="B21" s="48" t="s">
+      <c r="S20" s="57"/>
+      <c r="T20" s="57"/>
+      <c r="U20" s="57"/>
+      <c r="V20" s="57"/>
+      <c r="W20" s="57"/>
+      <c r="X20" s="57"/>
+      <c r="Y20" s="57"/>
+      <c r="Z20" s="57"/>
+    </row>
+    <row r="21" spans="2:26" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="C21" s="49" t="s">
+      <c r="C21" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="50" t="s">
+      <c r="D21" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="E21" s="34" t="s">
+      <c r="E21" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="F21" s="33" t="s">
+      <c r="F21" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="G21" s="50" t="s">
+      <c r="G21" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="H21" s="33" t="s">
+      <c r="H21" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="I21" s="19"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="17"/>
-      <c r="N21" s="17"/>
-      <c r="O21" s="16"/>
-      <c r="P21" s="16"/>
-      <c r="Q21" s="16"/>
-      <c r="R21" s="15"/>
-      <c r="S21" s="15"/>
-      <c r="T21" s="15"/>
-      <c r="U21" s="15"/>
-      <c r="V21" s="15"/>
-      <c r="W21" s="15"/>
-      <c r="X21" s="15"/>
-      <c r="Y21" s="15"/>
-      <c r="Z21" s="15"/>
-    </row>
-    <row r="22" spans="2:26" ht="19.899999999999999" customHeight="1">
-      <c r="B22" s="48" t="s">
+      <c r="I21" s="64"/>
+      <c r="J21" s="54"/>
+      <c r="K21" s="64"/>
+      <c r="L21" s="56"/>
+      <c r="M21" s="56"/>
+      <c r="N21" s="56"/>
+      <c r="O21" s="65"/>
+      <c r="P21" s="65"/>
+      <c r="Q21" s="65"/>
+      <c r="R21" s="57"/>
+      <c r="S21" s="57"/>
+      <c r="T21" s="57"/>
+      <c r="U21" s="57"/>
+      <c r="V21" s="57"/>
+      <c r="W21" s="57"/>
+      <c r="X21" s="57"/>
+      <c r="Y21" s="57"/>
+      <c r="Z21" s="57"/>
+    </row>
+    <row r="22" spans="2:26" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B22" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="C22" s="49" t="s">
+      <c r="C22" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="50" t="s">
+      <c r="D22" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="E22" s="34" t="s">
+      <c r="E22" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="F22" s="33" t="s">
+      <c r="F22" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="G22" s="50" t="s">
+      <c r="G22" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="H22" s="33" t="s">
+      <c r="H22" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="I22" s="19" t="s">
+      <c r="I22" s="64" t="s">
         <v>117</v>
       </c>
-      <c r="J22" s="18" t="s">
+      <c r="J22" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="K22" s="19" t="s">
+      <c r="K22" s="64" t="s">
         <v>129</v>
       </c>
-      <c r="L22" s="17" t="s">
+      <c r="L22" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="M22" s="17" t="s">
+      <c r="M22" s="56" t="s">
         <v>130</v>
       </c>
-      <c r="N22" s="17" t="s">
+      <c r="N22" s="56" t="s">
         <v>79</v>
       </c>
-      <c r="O22" s="16" t="s">
+      <c r="O22" s="65" t="s">
         <v>93</v>
       </c>
-      <c r="P22" s="16" t="s">
+      <c r="P22" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="Q22" s="16" t="s">
+      <c r="Q22" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="R22" s="15" t="s">
+      <c r="R22" s="57" t="s">
         <v>131</v>
       </c>
-      <c r="S22" s="15"/>
-      <c r="T22" s="15"/>
-      <c r="U22" s="15"/>
-      <c r="V22" s="15"/>
-      <c r="W22" s="15"/>
-      <c r="X22" s="15"/>
-      <c r="Y22" s="15"/>
-      <c r="Z22" s="15"/>
-    </row>
-    <row r="23" spans="2:26" ht="19.899999999999999" customHeight="1">
-      <c r="B23" s="48" t="s">
+      <c r="S22" s="57"/>
+      <c r="T22" s="57"/>
+      <c r="U22" s="57"/>
+      <c r="V22" s="57"/>
+      <c r="W22" s="57"/>
+      <c r="X22" s="57"/>
+      <c r="Y22" s="57"/>
+      <c r="Z22" s="57"/>
+    </row>
+    <row r="23" spans="2:26" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B23" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="C23" s="49" t="s">
+      <c r="C23" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="50" t="s">
+      <c r="D23" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="E23" s="34" t="s">
+      <c r="E23" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="F23" s="33" t="s">
+      <c r="F23" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="G23" s="50" t="s">
+      <c r="G23" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="H23" s="33" t="s">
+      <c r="H23" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="I23" s="19"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="17"/>
-      <c r="N23" s="17"/>
-      <c r="O23" s="16"/>
-      <c r="P23" s="16"/>
-      <c r="Q23" s="16"/>
-      <c r="R23" s="15"/>
-      <c r="S23" s="15"/>
-      <c r="T23" s="15"/>
-      <c r="U23" s="15"/>
-      <c r="V23" s="15"/>
-      <c r="W23" s="15"/>
-      <c r="X23" s="15"/>
-      <c r="Y23" s="15"/>
-      <c r="Z23" s="15"/>
-    </row>
-    <row r="24" spans="2:26" ht="19.899999999999999" customHeight="1">
-      <c r="B24" s="48" t="s">
+      <c r="I23" s="64"/>
+      <c r="J23" s="54"/>
+      <c r="K23" s="64"/>
+      <c r="L23" s="56"/>
+      <c r="M23" s="56"/>
+      <c r="N23" s="56"/>
+      <c r="O23" s="65"/>
+      <c r="P23" s="65"/>
+      <c r="Q23" s="65"/>
+      <c r="R23" s="57"/>
+      <c r="S23" s="57"/>
+      <c r="T23" s="57"/>
+      <c r="U23" s="57"/>
+      <c r="V23" s="57"/>
+      <c r="W23" s="57"/>
+      <c r="X23" s="57"/>
+      <c r="Y23" s="57"/>
+      <c r="Z23" s="57"/>
+    </row>
+    <row r="24" spans="2:26" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B24" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="C24" s="49" t="s">
+      <c r="C24" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="50" t="s">
+      <c r="D24" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="E24" s="34" t="s">
+      <c r="E24" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="F24" s="33" t="s">
+      <c r="F24" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="G24" s="50" t="s">
+      <c r="G24" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="H24" s="33" t="s">
+      <c r="H24" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="I24" s="19" t="s">
+      <c r="I24" s="64" t="s">
         <v>129</v>
       </c>
-      <c r="J24" s="18" t="s">
+      <c r="J24" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="K24" s="19" t="s">
+      <c r="K24" s="64" t="s">
         <v>141</v>
       </c>
-      <c r="L24" s="17" t="s">
+      <c r="L24" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="M24" s="17" t="s">
+      <c r="M24" s="56" t="s">
         <v>130</v>
       </c>
-      <c r="N24" s="17" t="s">
+      <c r="N24" s="56" t="s">
         <v>79</v>
       </c>
-      <c r="O24" s="16" t="s">
+      <c r="O24" s="65" t="s">
         <v>93</v>
       </c>
-      <c r="P24" s="16" t="s">
+      <c r="P24" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="Q24" s="16" t="s">
+      <c r="Q24" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="R24" s="15" t="s">
+      <c r="R24" s="57" t="s">
         <v>142</v>
       </c>
-      <c r="S24" s="15"/>
-      <c r="T24" s="15"/>
-      <c r="U24" s="15"/>
-      <c r="V24" s="15"/>
-      <c r="W24" s="15"/>
-      <c r="X24" s="15"/>
-      <c r="Y24" s="15"/>
-      <c r="Z24" s="15"/>
-    </row>
-    <row r="25" spans="2:26" ht="19.899999999999999" customHeight="1">
-      <c r="B25" s="48" t="s">
+      <c r="S24" s="57"/>
+      <c r="T24" s="57"/>
+      <c r="U24" s="57"/>
+      <c r="V24" s="57"/>
+      <c r="W24" s="57"/>
+      <c r="X24" s="57"/>
+      <c r="Y24" s="57"/>
+      <c r="Z24" s="57"/>
+    </row>
+    <row r="25" spans="2:26" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B25" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="C25" s="49" t="s">
+      <c r="C25" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="50" t="s">
+      <c r="D25" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="E25" s="34" t="s">
+      <c r="E25" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="F25" s="33" t="s">
+      <c r="F25" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="G25" s="50" t="s">
+      <c r="G25" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="H25" s="33" t="s">
+      <c r="H25" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="I25" s="19"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="17"/>
-      <c r="M25" s="17"/>
-      <c r="N25" s="17"/>
-      <c r="O25" s="16"/>
-      <c r="P25" s="16"/>
-      <c r="Q25" s="16"/>
-      <c r="R25" s="15"/>
-      <c r="S25" s="15"/>
-      <c r="T25" s="15"/>
-      <c r="U25" s="15"/>
-      <c r="V25" s="15"/>
-      <c r="W25" s="15"/>
-      <c r="X25" s="15"/>
-      <c r="Y25" s="15"/>
-      <c r="Z25" s="15"/>
-    </row>
-    <row r="26" spans="2:26" ht="19.899999999999999" customHeight="1">
-      <c r="B26" s="48" t="s">
+      <c r="I25" s="64"/>
+      <c r="J25" s="54"/>
+      <c r="K25" s="64"/>
+      <c r="L25" s="56"/>
+      <c r="M25" s="56"/>
+      <c r="N25" s="56"/>
+      <c r="O25" s="65"/>
+      <c r="P25" s="65"/>
+      <c r="Q25" s="65"/>
+      <c r="R25" s="57"/>
+      <c r="S25" s="57"/>
+      <c r="T25" s="57"/>
+      <c r="U25" s="57"/>
+      <c r="V25" s="57"/>
+      <c r="W25" s="57"/>
+      <c r="X25" s="57"/>
+      <c r="Y25" s="57"/>
+      <c r="Z25" s="57"/>
+    </row>
+    <row r="26" spans="2:26" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B26" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="C26" s="49" t="s">
+      <c r="C26" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="50" t="s">
+      <c r="D26" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="E26" s="34" t="s">
+      <c r="E26" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="F26" s="33" t="s">
+      <c r="F26" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="G26" s="50" t="s">
+      <c r="G26" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="H26" s="33" t="s">
+      <c r="H26" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="I26" s="76" t="s">
+      <c r="I26" s="58" t="s">
         <v>141</v>
       </c>
-      <c r="J26" s="77" t="s">
+      <c r="J26" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="K26" s="76" t="s">
+      <c r="K26" s="58" t="s">
         <v>153</v>
       </c>
-      <c r="L26" s="78" t="s">
+      <c r="L26" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="M26" s="78" t="s">
+      <c r="M26" s="61" t="s">
         <v>154</v>
       </c>
-      <c r="N26" s="78" t="s">
+      <c r="N26" s="61" t="s">
         <v>67</v>
       </c>
-      <c r="O26" s="79" t="s">
+      <c r="O26" s="62" t="s">
         <v>118</v>
       </c>
-      <c r="P26" s="79" t="s">
+      <c r="P26" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="Q26" s="79" t="s">
+      <c r="Q26" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="R26" s="15" t="s">
+      <c r="R26" s="57" t="s">
         <v>155</v>
       </c>
-      <c r="S26" s="15"/>
-      <c r="T26" s="15"/>
-      <c r="U26" s="15"/>
-      <c r="V26" s="15"/>
-      <c r="W26" s="15"/>
-      <c r="X26" s="15"/>
-      <c r="Y26" s="15"/>
-      <c r="Z26" s="15"/>
-    </row>
-    <row r="27" spans="2:26" ht="19.899999999999999" customHeight="1">
-      <c r="B27" s="48" t="s">
+      <c r="S26" s="57"/>
+      <c r="T26" s="57"/>
+      <c r="U26" s="57"/>
+      <c r="V26" s="57"/>
+      <c r="W26" s="57"/>
+      <c r="X26" s="57"/>
+      <c r="Y26" s="57"/>
+      <c r="Z26" s="57"/>
+    </row>
+    <row r="27" spans="2:26" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B27" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="C27" s="49" t="s">
+      <c r="C27" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="50" t="s">
+      <c r="D27" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="E27" s="34"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="50" t="s">
+      <c r="E27" s="5"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="H27" s="33" t="s">
+      <c r="H27" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="I27" s="76"/>
-      <c r="J27" s="77"/>
-      <c r="K27" s="76"/>
-      <c r="L27" s="78"/>
-      <c r="M27" s="78"/>
-      <c r="N27" s="78"/>
-      <c r="O27" s="79"/>
-      <c r="P27" s="79"/>
-      <c r="Q27" s="79"/>
-      <c r="R27" s="15"/>
-      <c r="S27" s="15"/>
-      <c r="T27" s="15"/>
-      <c r="U27" s="15"/>
-      <c r="V27" s="15"/>
-      <c r="W27" s="15"/>
-      <c r="X27" s="15"/>
-      <c r="Y27" s="15"/>
-      <c r="Z27" s="15"/>
-    </row>
-    <row r="28" spans="2:26" ht="19.899999999999999" customHeight="1">
-      <c r="B28" s="48"/>
-      <c r="C28" s="49" t="s">
+      <c r="I27" s="58"/>
+      <c r="J27" s="59"/>
+      <c r="K27" s="58"/>
+      <c r="L27" s="61"/>
+      <c r="M27" s="61"/>
+      <c r="N27" s="61"/>
+      <c r="O27" s="62"/>
+      <c r="P27" s="62"/>
+      <c r="Q27" s="62"/>
+      <c r="R27" s="57"/>
+      <c r="S27" s="57"/>
+      <c r="T27" s="57"/>
+      <c r="U27" s="57"/>
+      <c r="V27" s="57"/>
+      <c r="W27" s="57"/>
+      <c r="X27" s="57"/>
+      <c r="Y27" s="57"/>
+      <c r="Z27" s="57"/>
+    </row>
+    <row r="28" spans="2:26" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B28" s="19"/>
+      <c r="C28" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D28" s="50"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="50" t="s">
+      <c r="D28" s="21"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="H28" s="33" t="s">
+      <c r="H28" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="I28" s="76" t="s">
+      <c r="I28" s="58" t="s">
         <v>153</v>
       </c>
-      <c r="J28" s="77" t="s">
+      <c r="J28" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="K28" s="80" t="s">
+      <c r="K28" s="60" t="s">
         <v>160</v>
       </c>
-      <c r="L28" s="78" t="s">
+      <c r="L28" s="61" t="s">
         <v>67</v>
       </c>
-      <c r="M28" s="78" t="s">
+      <c r="M28" s="61" t="s">
         <v>161</v>
       </c>
-      <c r="N28" s="78" t="s">
+      <c r="N28" s="61" t="s">
         <v>130</v>
       </c>
-      <c r="O28" s="78" t="s">
+      <c r="O28" s="61" t="s">
         <v>162</v>
       </c>
-      <c r="P28" s="78" t="s">
+      <c r="P28" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="Q28" s="79" t="s">
+      <c r="Q28" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="R28" s="81" t="s">
+      <c r="R28" s="63" t="s">
         <v>163</v>
       </c>
-      <c r="S28" s="81"/>
-      <c r="T28" s="81"/>
-      <c r="U28" s="81"/>
-      <c r="V28" s="81"/>
-      <c r="W28" s="81"/>
-      <c r="X28" s="81"/>
-      <c r="Y28" s="81"/>
-      <c r="Z28" s="81"/>
-    </row>
-    <row r="29" spans="2:26" ht="19.899999999999999" customHeight="1">
-      <c r="B29" s="48"/>
-      <c r="C29" s="49" t="s">
+      <c r="S28" s="63"/>
+      <c r="T28" s="63"/>
+      <c r="U28" s="63"/>
+      <c r="V28" s="63"/>
+      <c r="W28" s="63"/>
+      <c r="X28" s="63"/>
+      <c r="Y28" s="63"/>
+      <c r="Z28" s="63"/>
+    </row>
+    <row r="29" spans="2:26" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B29" s="19"/>
+      <c r="C29" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="50"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="50" t="s">
+      <c r="D29" s="21"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="H29" s="33" t="s">
+      <c r="H29" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="I29" s="76"/>
-      <c r="J29" s="77"/>
-      <c r="K29" s="80"/>
-      <c r="L29" s="78"/>
-      <c r="M29" s="78"/>
-      <c r="N29" s="78"/>
-      <c r="O29" s="78"/>
-      <c r="P29" s="78"/>
-      <c r="Q29" s="79"/>
-      <c r="R29" s="81"/>
-      <c r="S29" s="81"/>
-      <c r="T29" s="81"/>
-      <c r="U29" s="81"/>
-      <c r="V29" s="81"/>
-      <c r="W29" s="81"/>
-      <c r="X29" s="81"/>
-      <c r="Y29" s="81"/>
-      <c r="Z29" s="81"/>
-    </row>
-    <row r="30" spans="2:26" ht="19.899999999999999" customHeight="1">
-      <c r="B30" s="48"/>
-      <c r="C30" s="49" t="s">
+      <c r="I29" s="58"/>
+      <c r="J29" s="59"/>
+      <c r="K29" s="60"/>
+      <c r="L29" s="61"/>
+      <c r="M29" s="61"/>
+      <c r="N29" s="61"/>
+      <c r="O29" s="61"/>
+      <c r="P29" s="61"/>
+      <c r="Q29" s="62"/>
+      <c r="R29" s="63"/>
+      <c r="S29" s="63"/>
+      <c r="T29" s="63"/>
+      <c r="U29" s="63"/>
+      <c r="V29" s="63"/>
+      <c r="W29" s="63"/>
+      <c r="X29" s="63"/>
+      <c r="Y29" s="63"/>
+      <c r="Z29" s="63"/>
+    </row>
+    <row r="30" spans="2:26" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B30" s="19"/>
+      <c r="C30" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="50"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="50"/>
-      <c r="H30" s="52"/>
-      <c r="I30" s="82" t="s">
+      <c r="D30" s="21"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="53" t="s">
         <v>160</v>
       </c>
-      <c r="J30" s="18"/>
-      <c r="K30" s="83" t="s">
+      <c r="J30" s="54"/>
+      <c r="K30" s="55" t="s">
         <v>157</v>
       </c>
-      <c r="L30" s="17" t="s">
+      <c r="L30" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="M30" s="17" t="s">
+      <c r="M30" s="56" t="s">
         <v>165</v>
       </c>
-      <c r="N30" s="17" t="s">
+      <c r="N30" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="O30" s="17" t="s">
+      <c r="O30" s="56" t="s">
         <v>162</v>
       </c>
-      <c r="P30" s="17" t="s">
+      <c r="P30" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="Q30" s="17" t="s">
+      <c r="Q30" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="R30" s="8" t="s">
+      <c r="R30" s="47" t="s">
         <v>166</v>
       </c>
-      <c r="S30" s="8"/>
-      <c r="T30" s="8"/>
-      <c r="U30" s="8"/>
-      <c r="V30" s="8"/>
-      <c r="W30" s="8"/>
-      <c r="X30" s="8"/>
-      <c r="Y30" s="8"/>
-      <c r="Z30" s="8"/>
-    </row>
-    <row r="31" spans="2:26" ht="19.899999999999999" customHeight="1">
-      <c r="B31" s="48"/>
-      <c r="C31" s="49" t="s">
+      <c r="S30" s="47"/>
+      <c r="T30" s="47"/>
+      <c r="U30" s="47"/>
+      <c r="V30" s="47"/>
+      <c r="W30" s="47"/>
+      <c r="X30" s="47"/>
+      <c r="Y30" s="47"/>
+      <c r="Z30" s="47"/>
+    </row>
+    <row r="31" spans="2:26" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B31" s="19"/>
+      <c r="C31" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D31" s="50"/>
-      <c r="E31" s="34"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="50"/>
-      <c r="H31" s="52"/>
-      <c r="I31" s="82"/>
-      <c r="J31" s="18"/>
-      <c r="K31" s="83"/>
-      <c r="L31" s="17"/>
-      <c r="M31" s="17"/>
-      <c r="N31" s="17"/>
-      <c r="O31" s="17"/>
-      <c r="P31" s="17"/>
-      <c r="Q31" s="17"/>
-      <c r="R31" s="8"/>
-      <c r="S31" s="8"/>
-      <c r="T31" s="8"/>
-      <c r="U31" s="8"/>
-      <c r="V31" s="8"/>
-      <c r="W31" s="8"/>
-      <c r="X31" s="8"/>
-      <c r="Y31" s="8"/>
-      <c r="Z31" s="8"/>
-    </row>
-    <row r="32" spans="2:26" ht="19.899999999999999" customHeight="1">
-      <c r="B32" s="53"/>
-      <c r="C32" s="51" t="s">
+      <c r="D31" s="21"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="53"/>
+      <c r="J31" s="54"/>
+      <c r="K31" s="55"/>
+      <c r="L31" s="56"/>
+      <c r="M31" s="56"/>
+      <c r="N31" s="56"/>
+      <c r="O31" s="56"/>
+      <c r="P31" s="56"/>
+      <c r="Q31" s="56"/>
+      <c r="R31" s="47"/>
+      <c r="S31" s="47"/>
+      <c r="T31" s="47"/>
+      <c r="U31" s="47"/>
+      <c r="V31" s="47"/>
+      <c r="W31" s="47"/>
+      <c r="X31" s="47"/>
+      <c r="Y31" s="47"/>
+      <c r="Z31" s="47"/>
+    </row>
+    <row r="32" spans="2:26" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B32" s="24"/>
+      <c r="C32" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="54"/>
-      <c r="E32" s="55"/>
-      <c r="F32" s="56"/>
-      <c r="G32" s="54"/>
-      <c r="H32" s="57"/>
-      <c r="I32" s="84"/>
-      <c r="J32" s="85" t="s">
+      <c r="D32" s="25"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="48"/>
+      <c r="J32" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="K32" s="86"/>
-      <c r="L32" s="87"/>
-      <c r="M32" s="87"/>
-      <c r="N32" s="87"/>
-      <c r="O32" s="87"/>
-      <c r="P32" s="87"/>
-      <c r="Q32" s="87"/>
-      <c r="R32" s="88"/>
-      <c r="S32" s="88"/>
-      <c r="T32" s="88"/>
-      <c r="U32" s="88"/>
-      <c r="V32" s="88"/>
-      <c r="W32" s="88"/>
-      <c r="X32" s="88"/>
-      <c r="Y32" s="88"/>
-      <c r="Z32" s="88"/>
-    </row>
-    <row r="33" spans="2:26" ht="19.899999999999999" customHeight="1">
-      <c r="B33" s="60"/>
-      <c r="C33" s="61" t="s">
+      <c r="K32" s="50"/>
+      <c r="L32" s="51"/>
+      <c r="M32" s="51"/>
+      <c r="N32" s="51"/>
+      <c r="O32" s="51"/>
+      <c r="P32" s="51"/>
+      <c r="Q32" s="51"/>
+      <c r="R32" s="52"/>
+      <c r="S32" s="52"/>
+      <c r="T32" s="52"/>
+      <c r="U32" s="52"/>
+      <c r="V32" s="52"/>
+      <c r="W32" s="52"/>
+      <c r="X32" s="52"/>
+      <c r="Y32" s="52"/>
+      <c r="Z32" s="52"/>
+    </row>
+    <row r="33" spans="2:26" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B33" s="31"/>
+      <c r="C33" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="D33" s="58"/>
-      <c r="E33" s="62"/>
-      <c r="F33" s="59"/>
-      <c r="G33" s="58"/>
-      <c r="H33" s="63"/>
-      <c r="I33" s="84"/>
-      <c r="J33" s="85"/>
-      <c r="K33" s="86"/>
-      <c r="L33" s="87"/>
-      <c r="M33" s="87"/>
-      <c r="N33" s="87"/>
-      <c r="O33" s="87"/>
-      <c r="P33" s="87"/>
-      <c r="Q33" s="87"/>
-      <c r="R33" s="88"/>
-      <c r="S33" s="88"/>
-      <c r="T33" s="88"/>
-      <c r="U33" s="88"/>
-      <c r="V33" s="88"/>
-      <c r="W33" s="88"/>
-      <c r="X33" s="88"/>
-      <c r="Y33" s="88"/>
-      <c r="Z33" s="88"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="48"/>
+      <c r="J33" s="49"/>
+      <c r="K33" s="50"/>
+      <c r="L33" s="51"/>
+      <c r="M33" s="51"/>
+      <c r="N33" s="51"/>
+      <c r="O33" s="51"/>
+      <c r="P33" s="51"/>
+      <c r="Q33" s="51"/>
+      <c r="R33" s="52"/>
+      <c r="S33" s="52"/>
+      <c r="T33" s="52"/>
+      <c r="U33" s="52"/>
+      <c r="V33" s="52"/>
+      <c r="W33" s="52"/>
+      <c r="X33" s="52"/>
+      <c r="Y33" s="52"/>
+      <c r="Z33" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="153">
-    <mergeCell ref="R30:Z31"/>
-    <mergeCell ref="I32:I33"/>
-    <mergeCell ref="J32:J33"/>
-    <mergeCell ref="K32:K33"/>
-    <mergeCell ref="L32:L33"/>
-    <mergeCell ref="M32:M33"/>
-    <mergeCell ref="N32:N33"/>
-    <mergeCell ref="O32:O33"/>
-    <mergeCell ref="P32:P33"/>
-    <mergeCell ref="Q32:Q33"/>
-    <mergeCell ref="R32:Z33"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="J30:J31"/>
-    <mergeCell ref="K30:K31"/>
-    <mergeCell ref="L30:L31"/>
-    <mergeCell ref="M30:M31"/>
-    <mergeCell ref="N30:N31"/>
-    <mergeCell ref="O30:O31"/>
-    <mergeCell ref="P30:P31"/>
-    <mergeCell ref="Q30:Q31"/>
-    <mergeCell ref="R26:Z27"/>
-    <mergeCell ref="I28:I29"/>
-    <mergeCell ref="J28:J29"/>
-    <mergeCell ref="K28:K29"/>
-    <mergeCell ref="L28:L29"/>
-    <mergeCell ref="M28:M29"/>
-    <mergeCell ref="N28:N29"/>
-    <mergeCell ref="O28:O29"/>
-    <mergeCell ref="P28:P29"/>
-    <mergeCell ref="Q28:Q29"/>
-    <mergeCell ref="R28:Z29"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="L26:L27"/>
-    <mergeCell ref="M26:M27"/>
-    <mergeCell ref="N26:N27"/>
-    <mergeCell ref="O26:O27"/>
-    <mergeCell ref="P26:P27"/>
-    <mergeCell ref="Q26:Q27"/>
-    <mergeCell ref="R22:Z23"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="L24:L25"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="N24:N25"/>
-    <mergeCell ref="O24:O25"/>
-    <mergeCell ref="P24:P25"/>
-    <mergeCell ref="Q24:Q25"/>
-    <mergeCell ref="R24:Z25"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="O22:O23"/>
-    <mergeCell ref="P22:P23"/>
-    <mergeCell ref="Q22:Q23"/>
-    <mergeCell ref="R18:Z19"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="J20:J21"/>
-    <mergeCell ref="K20:K21"/>
-    <mergeCell ref="L20:L21"/>
-    <mergeCell ref="M20:M21"/>
-    <mergeCell ref="N20:N21"/>
-    <mergeCell ref="O20:O21"/>
-    <mergeCell ref="P20:P21"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="R20:Z21"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="N18:N19"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="P18:P19"/>
-    <mergeCell ref="Q18:Q19"/>
-    <mergeCell ref="R14:Z15"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="O16:O17"/>
-    <mergeCell ref="P16:P17"/>
-    <mergeCell ref="Q16:Q17"/>
-    <mergeCell ref="R16:Z17"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="O14:O15"/>
-    <mergeCell ref="P14:P15"/>
-    <mergeCell ref="Q14:Q15"/>
-    <mergeCell ref="R10:Z11"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="M12:M13"/>
-    <mergeCell ref="N12:N13"/>
-    <mergeCell ref="O12:O13"/>
-    <mergeCell ref="P12:P13"/>
-    <mergeCell ref="Q12:Q13"/>
-    <mergeCell ref="R12:Z13"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="N10:N11"/>
-    <mergeCell ref="O10:O11"/>
-    <mergeCell ref="P10:P11"/>
-    <mergeCell ref="Q10:Q11"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:Q7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="R8:Z9"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="H1:L1"/>
     <mergeCell ref="M1:Q1"/>
@@ -4199,6 +4085,135 @@
     <mergeCell ref="M6:N6"/>
     <mergeCell ref="O6:Q6"/>
     <mergeCell ref="B7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:Q7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="R8:Z9"/>
+    <mergeCell ref="R10:Z11"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="N12:N13"/>
+    <mergeCell ref="O12:O13"/>
+    <mergeCell ref="P12:P13"/>
+    <mergeCell ref="Q12:Q13"/>
+    <mergeCell ref="R12:Z13"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="N10:N11"/>
+    <mergeCell ref="O10:O11"/>
+    <mergeCell ref="P10:P11"/>
+    <mergeCell ref="Q10:Q11"/>
+    <mergeCell ref="R14:Z15"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="P16:P17"/>
+    <mergeCell ref="Q16:Q17"/>
+    <mergeCell ref="R16:Z17"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="O14:O15"/>
+    <mergeCell ref="P14:P15"/>
+    <mergeCell ref="Q14:Q15"/>
+    <mergeCell ref="R18:Z19"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="L20:L21"/>
+    <mergeCell ref="M20:M21"/>
+    <mergeCell ref="N20:N21"/>
+    <mergeCell ref="O20:O21"/>
+    <mergeCell ref="P20:P21"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="R20:Z21"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="P18:P19"/>
+    <mergeCell ref="Q18:Q19"/>
+    <mergeCell ref="R22:Z23"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="N24:N25"/>
+    <mergeCell ref="O24:O25"/>
+    <mergeCell ref="P24:P25"/>
+    <mergeCell ref="Q24:Q25"/>
+    <mergeCell ref="R24:Z25"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="O22:O23"/>
+    <mergeCell ref="P22:P23"/>
+    <mergeCell ref="Q22:Q23"/>
+    <mergeCell ref="R26:Z27"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="J28:J29"/>
+    <mergeCell ref="K28:K29"/>
+    <mergeCell ref="L28:L29"/>
+    <mergeCell ref="M28:M29"/>
+    <mergeCell ref="N28:N29"/>
+    <mergeCell ref="O28:O29"/>
+    <mergeCell ref="P28:P29"/>
+    <mergeCell ref="Q28:Q29"/>
+    <mergeCell ref="R28:Z29"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="M26:M27"/>
+    <mergeCell ref="N26:N27"/>
+    <mergeCell ref="O26:O27"/>
+    <mergeCell ref="P26:P27"/>
+    <mergeCell ref="Q26:Q27"/>
+    <mergeCell ref="R30:Z31"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="J32:J33"/>
+    <mergeCell ref="K32:K33"/>
+    <mergeCell ref="L32:L33"/>
+    <mergeCell ref="M32:M33"/>
+    <mergeCell ref="N32:N33"/>
+    <mergeCell ref="O32:O33"/>
+    <mergeCell ref="P32:P33"/>
+    <mergeCell ref="Q32:Q33"/>
+    <mergeCell ref="R32:Z33"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="L30:L31"/>
+    <mergeCell ref="M30:M31"/>
+    <mergeCell ref="N30:N31"/>
+    <mergeCell ref="O30:O31"/>
+    <mergeCell ref="P30:P31"/>
+    <mergeCell ref="Q30:Q31"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.5" right="0.25" top="0.5" bottom="0.25" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -4208,878 +4223,836 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK26"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2:Q4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="1.140625" style="30" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" style="30" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" style="30" customWidth="1"/>
-    <col min="4" max="4" width="3.5703125" style="30" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" style="30" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" style="30" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" style="30" customWidth="1"/>
-    <col min="8" max="8" width="3.5703125" style="30" customWidth="1"/>
-    <col min="9" max="9" width="17" style="30" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" style="30" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" style="30" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" style="30" customWidth="1"/>
-    <col min="13" max="13" width="6.140625" style="30" customWidth="1"/>
-    <col min="14" max="14" width="10.28515625" style="30" customWidth="1"/>
-    <col min="15" max="15" width="6.140625" style="30" customWidth="1"/>
-    <col min="16" max="16" width="10.140625" style="30" customWidth="1"/>
-    <col min="17" max="17" width="3.5703125" style="30" customWidth="1"/>
-    <col min="18" max="1025" width="8.28515625" style="30" customWidth="1"/>
+    <col min="1" max="1" width="1.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="3.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="3.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="6.1640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.33203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="6.1640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="10.1640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="3.5" style="1" customWidth="1"/>
+    <col min="18" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.95" customHeight="1">
-      <c r="A1" s="89" t="s">
+    <row r="1" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="110" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="90" t="s">
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
+      <c r="D1" s="110"/>
+      <c r="E1" s="111" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="91" t="s">
+      <c r="F1" s="111"/>
+      <c r="G1" s="111"/>
+      <c r="H1" s="111"/>
+      <c r="I1" s="112" t="s">
         <v>167</v>
       </c>
-      <c r="J1" s="91"/>
-      <c r="K1" s="91"/>
-      <c r="L1" s="91"/>
-      <c r="M1" s="91"/>
-      <c r="N1" s="91"/>
-      <c r="O1" s="91"/>
-      <c r="P1" s="91"/>
-      <c r="Q1" s="91"/>
-    </row>
-    <row r="2" spans="1:17" ht="24.95" customHeight="1">
-      <c r="A2" s="92" t="s">
+      <c r="J1" s="112"/>
+      <c r="K1" s="112"/>
+      <c r="L1" s="112"/>
+      <c r="M1" s="112"/>
+      <c r="N1" s="112"/>
+      <c r="O1" s="112"/>
+      <c r="P1" s="112"/>
+      <c r="Q1" s="112"/>
+    </row>
+    <row r="2" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="108" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="93" t="s">
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="109" t="s">
         <v>169</v>
       </c>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="93"/>
-      <c r="I2" s="94" t="s">
+      <c r="F2" s="109"/>
+      <c r="G2" s="109"/>
+      <c r="H2" s="109"/>
+      <c r="I2" s="113" t="s">
         <v>262</v>
       </c>
-      <c r="J2" s="94"/>
-      <c r="K2" s="94"/>
-      <c r="L2" s="94"/>
-      <c r="M2" s="94"/>
-      <c r="N2" s="94"/>
-      <c r="O2" s="94"/>
-      <c r="P2" s="94"/>
-      <c r="Q2" s="94"/>
-    </row>
-    <row r="3" spans="1:17" ht="15" customHeight="1">
-      <c r="A3" s="95" t="s">
+      <c r="J2" s="113"/>
+      <c r="K2" s="113"/>
+      <c r="L2" s="113"/>
+      <c r="M2" s="113"/>
+      <c r="N2" s="113"/>
+      <c r="O2" s="113"/>
+      <c r="P2" s="113"/>
+      <c r="Q2" s="113"/>
+    </row>
+    <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="104" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="95"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="96" t="s">
+      <c r="B3" s="104"/>
+      <c r="C3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="114" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="94"/>
-      <c r="J3" s="94"/>
-      <c r="K3" s="94"/>
-      <c r="L3" s="94"/>
-      <c r="M3" s="94"/>
-      <c r="N3" s="94"/>
-      <c r="O3" s="94"/>
-      <c r="P3" s="94"/>
-      <c r="Q3" s="94"/>
-    </row>
-    <row r="4" spans="1:17" ht="27" customHeight="1">
-      <c r="A4" s="92" t="s">
+      <c r="F3" s="114"/>
+      <c r="G3" s="114"/>
+      <c r="H3" s="114"/>
+      <c r="I3" s="113"/>
+      <c r="J3" s="113"/>
+      <c r="K3" s="113"/>
+      <c r="L3" s="113"/>
+      <c r="M3" s="113"/>
+      <c r="N3" s="113"/>
+      <c r="O3" s="113"/>
+      <c r="P3" s="113"/>
+      <c r="Q3" s="113"/>
+    </row>
+    <row r="4" spans="1:17" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="108" t="s">
         <v>170</v>
       </c>
-      <c r="B4" s="92"/>
-      <c r="C4" s="92"/>
-      <c r="D4" s="92"/>
-      <c r="E4" s="97" t="s">
+      <c r="B4" s="108"/>
+      <c r="C4" s="108"/>
+      <c r="D4" s="108"/>
+      <c r="E4" s="115" t="s">
         <v>171</v>
       </c>
-      <c r="F4" s="97"/>
-      <c r="G4" s="97"/>
-      <c r="H4" s="97"/>
-      <c r="I4" s="94"/>
-      <c r="J4" s="94"/>
-      <c r="K4" s="94"/>
-      <c r="L4" s="94"/>
-      <c r="M4" s="94"/>
-      <c r="N4" s="94"/>
-      <c r="O4" s="94"/>
-      <c r="P4" s="94"/>
-      <c r="Q4" s="94"/>
-    </row>
-    <row r="5" spans="1:17" ht="15" customHeight="1">
-      <c r="A5" s="95" t="s">
+      <c r="F4" s="115"/>
+      <c r="G4" s="115"/>
+      <c r="H4" s="115"/>
+      <c r="I4" s="113"/>
+      <c r="J4" s="113"/>
+      <c r="K4" s="113"/>
+      <c r="L4" s="113"/>
+      <c r="M4" s="113"/>
+      <c r="N4" s="113"/>
+      <c r="O4" s="113"/>
+      <c r="P4" s="113"/>
+      <c r="Q4" s="113"/>
+    </row>
+    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="104" t="s">
         <v>172</v>
       </c>
-      <c r="B5" s="95"/>
-      <c r="C5" s="95"/>
-      <c r="D5" s="95"/>
-      <c r="E5" s="98" t="s">
+      <c r="B5" s="104"/>
+      <c r="C5" s="104"/>
+      <c r="D5" s="104"/>
+      <c r="E5" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="98"/>
-      <c r="G5" s="98"/>
-      <c r="H5" s="98"/>
-      <c r="I5" s="99" t="s">
+      <c r="F5" s="105"/>
+      <c r="G5" s="105"/>
+      <c r="H5" s="105"/>
+      <c r="I5" s="100" t="s">
         <v>173</v>
       </c>
-      <c r="J5" s="100"/>
-      <c r="K5" s="101" t="s">
+      <c r="J5" s="106"/>
+      <c r="K5" s="107" t="s">
         <v>174</v>
       </c>
-      <c r="L5" s="100"/>
-      <c r="M5" s="100"/>
-      <c r="N5" s="100"/>
-      <c r="O5" s="100"/>
-      <c r="P5" s="102"/>
-      <c r="Q5" s="102"/>
-    </row>
-    <row r="6" spans="1:17" ht="24" customHeight="1">
-      <c r="A6" s="92" t="s">
+      <c r="L5" s="106"/>
+      <c r="M5" s="106"/>
+      <c r="N5" s="106"/>
+      <c r="O5" s="106"/>
+      <c r="P5" s="96"/>
+      <c r="Q5" s="96"/>
+    </row>
+    <row r="6" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="108" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="92"/>
-      <c r="C6" s="92"/>
-      <c r="D6" s="92"/>
-      <c r="E6" s="93" t="s">
+      <c r="B6" s="108"/>
+      <c r="C6" s="108"/>
+      <c r="D6" s="108"/>
+      <c r="E6" s="109" t="s">
         <v>175</v>
       </c>
-      <c r="F6" s="93"/>
-      <c r="G6" s="93"/>
-      <c r="H6" s="93"/>
-      <c r="I6" s="99"/>
-      <c r="J6" s="100"/>
-      <c r="K6" s="101"/>
-      <c r="L6" s="100"/>
-      <c r="M6" s="100"/>
-      <c r="N6" s="100"/>
-      <c r="O6" s="100"/>
-      <c r="P6" s="102"/>
-      <c r="Q6" s="102"/>
-    </row>
-    <row r="7" spans="1:17" ht="25.15" customHeight="1">
-      <c r="A7" s="103" t="s">
+      <c r="F6" s="109"/>
+      <c r="G6" s="109"/>
+      <c r="H6" s="109"/>
+      <c r="I6" s="100"/>
+      <c r="J6" s="106"/>
+      <c r="K6" s="107"/>
+      <c r="L6" s="106"/>
+      <c r="M6" s="106"/>
+      <c r="N6" s="106"/>
+      <c r="O6" s="106"/>
+      <c r="P6" s="96"/>
+      <c r="Q6" s="96"/>
+    </row>
+    <row r="7" spans="1:17" ht="25.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="102" t="s">
         <v>176</v>
       </c>
-      <c r="B7" s="104" t="s">
+      <c r="B7" s="90" t="s">
         <v>177</v>
       </c>
-      <c r="C7" s="104"/>
-      <c r="D7" s="47" t="s">
+      <c r="C7" s="90"/>
+      <c r="D7" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="104" t="s">
+      <c r="E7" s="90" t="s">
         <v>178</v>
       </c>
-      <c r="F7" s="104"/>
-      <c r="G7" s="104"/>
-      <c r="H7" s="47" t="s">
+      <c r="F7" s="90"/>
+      <c r="G7" s="90"/>
+      <c r="H7" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="I7" s="64" t="s">
+      <c r="I7" s="35" t="s">
         <v>179</v>
       </c>
-      <c r="J7" s="47"/>
-      <c r="K7" s="47" t="s">
+      <c r="J7" s="18"/>
+      <c r="K7" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="L7" s="104"/>
-      <c r="M7" s="104"/>
-      <c r="N7" s="104"/>
-      <c r="O7" s="104"/>
-      <c r="P7" s="102"/>
-      <c r="Q7" s="102"/>
-    </row>
-    <row r="8" spans="1:17" ht="25.15" customHeight="1">
-      <c r="A8" s="103"/>
-      <c r="B8" s="104" t="s">
+      <c r="L7" s="90"/>
+      <c r="M7" s="90"/>
+      <c r="N7" s="90"/>
+      <c r="O7" s="90"/>
+      <c r="P7" s="96"/>
+      <c r="Q7" s="96"/>
+    </row>
+    <row r="8" spans="1:17" ht="25.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="102"/>
+      <c r="B8" s="90" t="s">
         <v>181</v>
       </c>
-      <c r="C8" s="104"/>
-      <c r="D8" s="47" t="s">
+      <c r="C8" s="90"/>
+      <c r="D8" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="104" t="s">
+      <c r="E8" s="90" t="s">
         <v>182</v>
       </c>
-      <c r="F8" s="104"/>
-      <c r="G8" s="104"/>
-      <c r="H8" s="47" t="s">
+      <c r="F8" s="90"/>
+      <c r="G8" s="90"/>
+      <c r="H8" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="I8" s="64" t="s">
+      <c r="I8" s="35" t="s">
         <v>183</v>
       </c>
-      <c r="J8" s="47" t="s">
+      <c r="J8" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="K8" s="47"/>
-      <c r="L8" s="104"/>
-      <c r="M8" s="104"/>
-      <c r="N8" s="104"/>
-      <c r="O8" s="104"/>
-      <c r="P8" s="102"/>
-      <c r="Q8" s="102"/>
-    </row>
-    <row r="9" spans="1:17" ht="25.15" customHeight="1">
-      <c r="A9" s="103"/>
-      <c r="B9" s="104" t="s">
+      <c r="K8" s="18"/>
+      <c r="L8" s="90"/>
+      <c r="M8" s="90"/>
+      <c r="N8" s="90"/>
+      <c r="O8" s="90"/>
+      <c r="P8" s="96"/>
+      <c r="Q8" s="96"/>
+    </row>
+    <row r="9" spans="1:17" ht="25.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="102"/>
+      <c r="B9" s="90" t="s">
         <v>185</v>
       </c>
-      <c r="C9" s="104"/>
-      <c r="D9" s="47" t="s">
+      <c r="C9" s="90"/>
+      <c r="D9" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="104" t="s">
+      <c r="E9" s="90" t="s">
         <v>186</v>
       </c>
-      <c r="F9" s="104"/>
-      <c r="G9" s="104"/>
-      <c r="H9" s="47" t="s">
+      <c r="F9" s="90"/>
+      <c r="G9" s="90"/>
+      <c r="H9" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="I9" s="47" t="s">
+      <c r="I9" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="J9" s="47"/>
-      <c r="K9" s="47"/>
-      <c r="L9" s="104" t="s">
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="90" t="s">
         <v>188</v>
       </c>
-      <c r="M9" s="104"/>
-      <c r="N9" s="105"/>
-      <c r="O9" s="105"/>
-      <c r="P9" s="106"/>
-      <c r="Q9" s="106"/>
-    </row>
-    <row r="10" spans="1:17" ht="25.15" customHeight="1">
-      <c r="A10" s="103"/>
-      <c r="B10" s="104" t="s">
+      <c r="M9" s="90"/>
+      <c r="N9" s="103"/>
+      <c r="O9" s="103"/>
+      <c r="P9" s="101"/>
+      <c r="Q9" s="101"/>
+    </row>
+    <row r="10" spans="1:17" ht="25.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="102"/>
+      <c r="B10" s="90" t="s">
         <v>189</v>
       </c>
-      <c r="C10" s="104"/>
-      <c r="D10" s="47" t="s">
+      <c r="C10" s="90"/>
+      <c r="D10" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="E10" s="104" t="s">
+      <c r="E10" s="90" t="s">
         <v>190</v>
       </c>
-      <c r="F10" s="104"/>
-      <c r="G10" s="104"/>
-      <c r="H10" s="47" t="s">
+      <c r="F10" s="90"/>
+      <c r="G10" s="90"/>
+      <c r="H10" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="I10" s="99" t="s">
+      <c r="I10" s="100" t="s">
         <v>191</v>
       </c>
-      <c r="J10" s="99"/>
-      <c r="K10" s="47" t="s">
+      <c r="J10" s="100"/>
+      <c r="K10" s="18" t="s">
         <v>192</v>
       </c>
-      <c r="L10" s="104"/>
-      <c r="M10" s="104"/>
-      <c r="N10" s="104"/>
-      <c r="O10" s="104"/>
-      <c r="P10" s="106"/>
-      <c r="Q10" s="106"/>
-    </row>
-    <row r="11" spans="1:17" ht="25.15" customHeight="1">
-      <c r="A11" s="103"/>
-      <c r="B11" s="104" t="s">
+      <c r="L10" s="90"/>
+      <c r="M10" s="90"/>
+      <c r="N10" s="90"/>
+      <c r="O10" s="90"/>
+      <c r="P10" s="101"/>
+      <c r="Q10" s="101"/>
+    </row>
+    <row r="11" spans="1:17" ht="25.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="102"/>
+      <c r="B11" s="90" t="s">
         <v>193</v>
       </c>
-      <c r="C11" s="104"/>
-      <c r="D11" s="47" t="s">
+      <c r="C11" s="90"/>
+      <c r="D11" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="104" t="s">
+      <c r="E11" s="90" t="s">
         <v>194</v>
       </c>
-      <c r="F11" s="104"/>
-      <c r="G11" s="104"/>
-      <c r="H11" s="47" t="s">
+      <c r="F11" s="90"/>
+      <c r="G11" s="90"/>
+      <c r="H11" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="I11" s="99" t="s">
+      <c r="I11" s="100" t="s">
         <v>195</v>
       </c>
-      <c r="J11" s="99"/>
-      <c r="K11" s="47" t="s">
+      <c r="J11" s="100"/>
+      <c r="K11" s="18" t="s">
         <v>196</v>
       </c>
-      <c r="L11" s="104"/>
-      <c r="M11" s="104"/>
-      <c r="N11" s="104"/>
-      <c r="O11" s="104"/>
-      <c r="P11" s="102"/>
-      <c r="Q11" s="102"/>
-    </row>
-    <row r="12" spans="1:17" ht="25.15" customHeight="1">
-      <c r="A12" s="103"/>
-      <c r="B12" s="104" t="s">
+      <c r="L11" s="90"/>
+      <c r="M11" s="90"/>
+      <c r="N11" s="90"/>
+      <c r="O11" s="90"/>
+      <c r="P11" s="96"/>
+      <c r="Q11" s="96"/>
+    </row>
+    <row r="12" spans="1:17" ht="25.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="102"/>
+      <c r="B12" s="90" t="s">
         <v>197</v>
       </c>
-      <c r="C12" s="104"/>
-      <c r="D12" s="47" t="s">
+      <c r="C12" s="90"/>
+      <c r="D12" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="E12" s="104" t="s">
+      <c r="E12" s="90" t="s">
         <v>198</v>
       </c>
-      <c r="F12" s="104"/>
-      <c r="G12" s="104"/>
-      <c r="H12" s="47" t="s">
+      <c r="F12" s="90"/>
+      <c r="G12" s="90"/>
+      <c r="H12" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="I12" s="99" t="s">
+      <c r="I12" s="100" t="s">
         <v>199</v>
       </c>
-      <c r="J12" s="99"/>
-      <c r="K12" s="47" t="s">
+      <c r="J12" s="100"/>
+      <c r="K12" s="18" t="s">
         <v>200</v>
       </c>
-      <c r="L12" s="104"/>
-      <c r="M12" s="104"/>
-      <c r="N12" s="104"/>
-      <c r="O12" s="104"/>
-      <c r="P12" s="106"/>
-      <c r="Q12" s="106"/>
-    </row>
-    <row r="13" spans="1:17" ht="25.15" customHeight="1">
-      <c r="A13" s="103"/>
-      <c r="B13" s="104" t="s">
+      <c r="L12" s="90"/>
+      <c r="M12" s="90"/>
+      <c r="N12" s="90"/>
+      <c r="O12" s="90"/>
+      <c r="P12" s="101"/>
+      <c r="Q12" s="101"/>
+    </row>
+    <row r="13" spans="1:17" ht="25.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="102"/>
+      <c r="B13" s="90" t="s">
         <v>201</v>
       </c>
-      <c r="C13" s="104"/>
-      <c r="D13" s="47" t="s">
+      <c r="C13" s="90"/>
+      <c r="D13" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="104" t="s">
+      <c r="E13" s="90" t="s">
         <v>202</v>
       </c>
-      <c r="F13" s="104"/>
-      <c r="G13" s="104"/>
-      <c r="H13" s="47" t="s">
+      <c r="F13" s="90"/>
+      <c r="G13" s="90"/>
+      <c r="H13" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="I13" s="99" t="s">
+      <c r="I13" s="100" t="s">
         <v>203</v>
       </c>
-      <c r="J13" s="99"/>
-      <c r="K13" s="47" t="s">
+      <c r="J13" s="100"/>
+      <c r="K13" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="L13" s="104" t="s">
+      <c r="L13" s="90" t="s">
         <v>205</v>
       </c>
-      <c r="M13" s="104"/>
-      <c r="N13" s="104" t="s">
+      <c r="M13" s="90"/>
+      <c r="N13" s="90" t="s">
         <v>206</v>
       </c>
-      <c r="O13" s="104"/>
-      <c r="P13" s="102"/>
-      <c r="Q13" s="102"/>
-    </row>
-    <row r="14" spans="1:17" ht="25.15" customHeight="1">
-      <c r="A14" s="103"/>
-      <c r="B14" s="104" t="s">
+      <c r="O13" s="90"/>
+      <c r="P13" s="96"/>
+      <c r="Q13" s="96"/>
+    </row>
+    <row r="14" spans="1:17" ht="25.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="102"/>
+      <c r="B14" s="90" t="s">
         <v>207</v>
       </c>
-      <c r="C14" s="104"/>
-      <c r="D14" s="47" t="s">
+      <c r="C14" s="90"/>
+      <c r="D14" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="104" t="s">
+      <c r="E14" s="90" t="s">
         <v>208</v>
       </c>
-      <c r="F14" s="104"/>
-      <c r="G14" s="104"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="99" t="s">
+      <c r="F14" s="90"/>
+      <c r="G14" s="90"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="100" t="s">
         <v>209</v>
       </c>
-      <c r="J14" s="99"/>
-      <c r="K14" s="99"/>
-      <c r="L14" s="47" t="s">
+      <c r="J14" s="100"/>
+      <c r="K14" s="100"/>
+      <c r="L14" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="M14" s="47" t="s">
+      <c r="M14" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="N14" s="47" t="s">
+      <c r="N14" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="O14" s="47" t="s">
+      <c r="O14" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="P14" s="47"/>
-      <c r="Q14" s="65" t="s">
+      <c r="P14" s="18"/>
+      <c r="Q14" s="36" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="32.1" customHeight="1">
-      <c r="A15" s="66">
+    <row r="15" spans="1:17" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="37">
         <v>1</v>
       </c>
-      <c r="B15" s="107" t="s">
+      <c r="B15" s="98" t="s">
         <v>211</v>
       </c>
-      <c r="C15" s="107"/>
-      <c r="D15" s="107"/>
-      <c r="E15" s="107"/>
-      <c r="F15" s="107"/>
-      <c r="G15" s="107"/>
-      <c r="H15" s="107"/>
-      <c r="I15" s="104" t="s">
+      <c r="C15" s="98"/>
+      <c r="D15" s="98"/>
+      <c r="E15" s="98"/>
+      <c r="F15" s="98"/>
+      <c r="G15" s="98"/>
+      <c r="H15" s="98"/>
+      <c r="I15" s="90" t="s">
         <v>212</v>
       </c>
-      <c r="J15" s="104"/>
-      <c r="K15" s="47" t="s">
+      <c r="J15" s="90"/>
+      <c r="K15" s="18" t="s">
         <v>213</v>
       </c>
-      <c r="L15" s="104"/>
-      <c r="M15" s="104"/>
-      <c r="N15" s="104"/>
-      <c r="O15" s="104"/>
-      <c r="P15" s="102"/>
-      <c r="Q15" s="102"/>
-    </row>
-    <row r="16" spans="1:17" ht="24" customHeight="1">
-      <c r="A16" s="67">
+      <c r="L15" s="90"/>
+      <c r="M15" s="90"/>
+      <c r="N15" s="90"/>
+      <c r="O15" s="90"/>
+      <c r="P15" s="96"/>
+      <c r="Q15" s="96"/>
+    </row>
+    <row r="16" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="38">
         <v>2</v>
       </c>
-      <c r="B16" s="108" t="s">
+      <c r="B16" s="89" t="s">
         <v>214</v>
       </c>
-      <c r="C16" s="108"/>
-      <c r="D16" s="108"/>
-      <c r="E16" s="108"/>
-      <c r="F16" s="108"/>
-      <c r="G16" s="108"/>
-      <c r="H16" s="108"/>
-      <c r="I16" s="108"/>
-      <c r="J16" s="109" t="s">
+      <c r="C16" s="89"/>
+      <c r="D16" s="89"/>
+      <c r="E16" s="89"/>
+      <c r="F16" s="89"/>
+      <c r="G16" s="89"/>
+      <c r="H16" s="89"/>
+      <c r="I16" s="89"/>
+      <c r="J16" s="99" t="s">
         <v>215</v>
       </c>
-      <c r="K16" s="109"/>
-      <c r="L16" s="109"/>
-      <c r="M16" s="109"/>
-      <c r="N16" s="109"/>
-      <c r="O16" s="109"/>
-      <c r="P16" s="109"/>
-      <c r="Q16" s="109"/>
-    </row>
-    <row r="17" spans="1:17" ht="22.15" customHeight="1">
-      <c r="A17" s="67">
+      <c r="K16" s="99"/>
+      <c r="L16" s="99"/>
+      <c r="M16" s="99"/>
+      <c r="N16" s="99"/>
+      <c r="O16" s="99"/>
+      <c r="P16" s="99"/>
+      <c r="Q16" s="99"/>
+    </row>
+    <row r="17" spans="1:17" ht="22.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="38">
         <v>3</v>
       </c>
-      <c r="B17" s="108" t="s">
+      <c r="B17" s="89" t="s">
         <v>216</v>
       </c>
-      <c r="C17" s="108"/>
-      <c r="D17" s="108"/>
-      <c r="E17" s="108"/>
-      <c r="F17" s="108"/>
-      <c r="G17" s="108"/>
-      <c r="H17" s="108"/>
-      <c r="I17" s="108"/>
-      <c r="J17" s="110" t="s">
+      <c r="C17" s="89"/>
+      <c r="D17" s="89"/>
+      <c r="E17" s="89"/>
+      <c r="F17" s="89"/>
+      <c r="G17" s="89"/>
+      <c r="H17" s="89"/>
+      <c r="I17" s="89"/>
+      <c r="J17" s="95" t="s">
         <v>217</v>
       </c>
-      <c r="K17" s="110"/>
-      <c r="L17" s="104" t="s">
+      <c r="K17" s="95"/>
+      <c r="L17" s="90" t="s">
         <v>218</v>
       </c>
-      <c r="M17" s="104"/>
-      <c r="N17" s="104" t="s">
+      <c r="M17" s="90"/>
+      <c r="N17" s="90" t="s">
         <v>219</v>
       </c>
-      <c r="O17" s="104"/>
-      <c r="P17" s="102" t="s">
+      <c r="O17" s="90"/>
+      <c r="P17" s="96" t="s">
         <v>220</v>
       </c>
-      <c r="Q17" s="102"/>
-    </row>
-    <row r="18" spans="1:17" ht="22.15" customHeight="1">
-      <c r="A18" s="67">
+      <c r="Q17" s="96"/>
+    </row>
+    <row r="18" spans="1:17" ht="22.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="38">
         <v>4</v>
       </c>
-      <c r="B18" s="108" t="s">
+      <c r="B18" s="89" t="s">
         <v>221</v>
       </c>
-      <c r="C18" s="108"/>
-      <c r="D18" s="108"/>
-      <c r="E18" s="108"/>
-      <c r="F18" s="108"/>
-      <c r="G18" s="108"/>
-      <c r="H18" s="108"/>
-      <c r="I18" s="108"/>
-      <c r="J18" s="110" t="s">
+      <c r="C18" s="89"/>
+      <c r="D18" s="89"/>
+      <c r="E18" s="89"/>
+      <c r="F18" s="89"/>
+      <c r="G18" s="89"/>
+      <c r="H18" s="89"/>
+      <c r="I18" s="89"/>
+      <c r="J18" s="95" t="s">
         <v>222</v>
       </c>
-      <c r="K18" s="110"/>
-      <c r="L18" s="104" t="s">
+      <c r="K18" s="95"/>
+      <c r="L18" s="90" t="s">
         <v>223</v>
       </c>
-      <c r="M18" s="104"/>
-      <c r="N18" s="104" t="s">
+      <c r="M18" s="90"/>
+      <c r="N18" s="90" t="s">
         <v>224</v>
       </c>
-      <c r="O18" s="104"/>
-      <c r="P18" s="102" t="s">
+      <c r="O18" s="90"/>
+      <c r="P18" s="96" t="s">
         <v>225</v>
       </c>
-      <c r="Q18" s="102"/>
-    </row>
-    <row r="19" spans="1:17" ht="22.15" customHeight="1">
-      <c r="A19" s="67">
+      <c r="Q18" s="96"/>
+    </row>
+    <row r="19" spans="1:17" ht="22.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="38">
         <v>5</v>
       </c>
-      <c r="B19" s="108" t="s">
+      <c r="B19" s="89" t="s">
         <v>226</v>
       </c>
-      <c r="C19" s="108"/>
-      <c r="D19" s="108"/>
-      <c r="E19" s="108"/>
-      <c r="F19" s="108"/>
-      <c r="G19" s="108"/>
-      <c r="H19" s="108"/>
-      <c r="I19" s="108"/>
-      <c r="J19" s="111" t="s">
+      <c r="C19" s="89"/>
+      <c r="D19" s="89"/>
+      <c r="E19" s="89"/>
+      <c r="F19" s="89"/>
+      <c r="G19" s="89"/>
+      <c r="H19" s="89"/>
+      <c r="I19" s="89"/>
+      <c r="J19" s="97" t="s">
         <v>227</v>
       </c>
-      <c r="K19" s="111"/>
-      <c r="L19" s="112" t="s">
+      <c r="K19" s="97"/>
+      <c r="L19" s="92" t="s">
         <v>207</v>
       </c>
-      <c r="M19" s="112"/>
-      <c r="N19" s="112"/>
-      <c r="O19" s="112"/>
-      <c r="P19" s="112"/>
-      <c r="Q19" s="112"/>
-    </row>
-    <row r="20" spans="1:17" ht="24" customHeight="1">
-      <c r="A20" s="67">
+      <c r="M19" s="92"/>
+      <c r="N19" s="92"/>
+      <c r="O19" s="92"/>
+      <c r="P19" s="92"/>
+      <c r="Q19" s="92"/>
+    </row>
+    <row r="20" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="38">
         <v>6</v>
       </c>
-      <c r="B20" s="108" t="s">
+      <c r="B20" s="89" t="s">
         <v>228</v>
       </c>
-      <c r="C20" s="108"/>
-      <c r="D20" s="108"/>
-      <c r="E20" s="108"/>
-      <c r="F20" s="108"/>
-      <c r="G20" s="108"/>
-      <c r="H20" s="108"/>
-      <c r="I20" s="108"/>
-      <c r="J20" s="68" t="s">
+      <c r="C20" s="89"/>
+      <c r="D20" s="89"/>
+      <c r="E20" s="89"/>
+      <c r="F20" s="89"/>
+      <c r="G20" s="89"/>
+      <c r="H20" s="89"/>
+      <c r="I20" s="89"/>
+      <c r="J20" s="39" t="s">
         <v>229</v>
       </c>
-      <c r="K20" s="69" t="s">
+      <c r="K20" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="L20" s="104" t="s">
+      <c r="L20" s="90" t="s">
         <v>196</v>
       </c>
-      <c r="M20" s="104"/>
-      <c r="N20" s="113" t="s">
+      <c r="M20" s="90"/>
+      <c r="N20" s="91" t="s">
         <v>230</v>
       </c>
-      <c r="O20" s="113"/>
-      <c r="P20" s="112" t="s">
+      <c r="O20" s="91"/>
+      <c r="P20" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="Q20" s="112"/>
-    </row>
-    <row r="21" spans="1:17" ht="24" customHeight="1">
-      <c r="A21" s="67">
+      <c r="Q20" s="92"/>
+    </row>
+    <row r="21" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="38">
         <v>7</v>
       </c>
-      <c r="B21" s="108" t="s">
+      <c r="B21" s="89" t="s">
         <v>231</v>
       </c>
-      <c r="C21" s="108"/>
-      <c r="D21" s="108"/>
-      <c r="E21" s="108"/>
-      <c r="F21" s="108"/>
-      <c r="G21" s="108"/>
-      <c r="H21" s="108"/>
-      <c r="I21" s="108"/>
-      <c r="J21" s="68" t="s">
+      <c r="C21" s="89"/>
+      <c r="D21" s="89"/>
+      <c r="E21" s="89"/>
+      <c r="F21" s="89"/>
+      <c r="G21" s="89"/>
+      <c r="H21" s="89"/>
+      <c r="I21" s="89"/>
+      <c r="J21" s="39" t="s">
         <v>232</v>
       </c>
-      <c r="K21" s="69" t="s">
+      <c r="K21" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="L21" s="104" t="s">
+      <c r="L21" s="90" t="s">
         <v>233</v>
       </c>
-      <c r="M21" s="104"/>
-      <c r="N21" s="113" t="s">
+      <c r="M21" s="90"/>
+      <c r="N21" s="91" t="s">
         <v>234</v>
       </c>
-      <c r="O21" s="113"/>
-      <c r="P21" s="112" t="s">
+      <c r="O21" s="91"/>
+      <c r="P21" s="92" t="s">
         <v>235</v>
       </c>
-      <c r="Q21" s="112"/>
-    </row>
-    <row r="22" spans="1:17" ht="24" customHeight="1">
-      <c r="A22" s="67">
+      <c r="Q21" s="92"/>
+    </row>
+    <row r="22" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="38">
         <v>8</v>
       </c>
-      <c r="B22" s="108" t="s">
+      <c r="B22" s="89" t="s">
         <v>236</v>
       </c>
-      <c r="C22" s="108"/>
-      <c r="D22" s="108"/>
-      <c r="E22" s="108"/>
-      <c r="F22" s="108"/>
-      <c r="G22" s="108"/>
-      <c r="H22" s="108"/>
-      <c r="I22" s="108"/>
-      <c r="J22" s="68" t="s">
+      <c r="C22" s="89"/>
+      <c r="D22" s="89"/>
+      <c r="E22" s="89"/>
+      <c r="F22" s="89"/>
+      <c r="G22" s="89"/>
+      <c r="H22" s="89"/>
+      <c r="I22" s="89"/>
+      <c r="J22" s="39" t="s">
         <v>237</v>
       </c>
-      <c r="K22" s="69" t="s">
+      <c r="K22" s="40" t="s">
         <v>162</v>
       </c>
-      <c r="L22" s="104" t="s">
+      <c r="L22" s="90" t="s">
         <v>238</v>
       </c>
-      <c r="M22" s="104"/>
-      <c r="N22" s="113" t="s">
+      <c r="M22" s="90"/>
+      <c r="N22" s="91" t="s">
         <v>239</v>
       </c>
-      <c r="O22" s="113"/>
-      <c r="P22" s="112" t="s">
+      <c r="O22" s="91"/>
+      <c r="P22" s="92" t="s">
         <v>240</v>
       </c>
-      <c r="Q22" s="112"/>
-    </row>
-    <row r="23" spans="1:17" ht="24" customHeight="1">
-      <c r="A23" s="67">
+      <c r="Q22" s="92"/>
+    </row>
+    <row r="23" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="38">
         <v>9</v>
       </c>
-      <c r="B23" s="108" t="s">
+      <c r="B23" s="89" t="s">
         <v>241</v>
       </c>
-      <c r="C23" s="108"/>
-      <c r="D23" s="108"/>
-      <c r="E23" s="108"/>
-      <c r="F23" s="108"/>
-      <c r="G23" s="108"/>
-      <c r="H23" s="108"/>
-      <c r="I23" s="108"/>
-      <c r="J23" s="68" t="s">
+      <c r="C23" s="89"/>
+      <c r="D23" s="89"/>
+      <c r="E23" s="89"/>
+      <c r="F23" s="89"/>
+      <c r="G23" s="89"/>
+      <c r="H23" s="89"/>
+      <c r="I23" s="89"/>
+      <c r="J23" s="39" t="s">
         <v>242</v>
       </c>
-      <c r="K23" s="69" t="s">
+      <c r="K23" s="40" t="s">
         <v>235</v>
       </c>
-      <c r="L23" s="104" t="s">
+      <c r="L23" s="90" t="s">
         <v>243</v>
       </c>
-      <c r="M23" s="104"/>
-      <c r="N23" s="113" t="s">
+      <c r="M23" s="90"/>
+      <c r="N23" s="91" t="s">
         <v>244</v>
       </c>
-      <c r="O23" s="113"/>
-      <c r="P23" s="112" t="s">
+      <c r="O23" s="91"/>
+      <c r="P23" s="92" t="s">
         <v>245</v>
       </c>
-      <c r="Q23" s="112"/>
-    </row>
-    <row r="24" spans="1:17" ht="24" customHeight="1">
-      <c r="A24" s="67">
+      <c r="Q23" s="92"/>
+    </row>
+    <row r="24" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="38">
         <v>10</v>
       </c>
-      <c r="B24" s="108" t="s">
+      <c r="B24" s="89" t="s">
         <v>246</v>
       </c>
-      <c r="C24" s="108"/>
-      <c r="D24" s="108"/>
-      <c r="E24" s="108"/>
-      <c r="F24" s="108"/>
-      <c r="G24" s="108"/>
-      <c r="H24" s="108"/>
-      <c r="I24" s="108"/>
-      <c r="J24" s="68" t="s">
+      <c r="C24" s="89"/>
+      <c r="D24" s="89"/>
+      <c r="E24" s="89"/>
+      <c r="F24" s="89"/>
+      <c r="G24" s="89"/>
+      <c r="H24" s="89"/>
+      <c r="I24" s="89"/>
+      <c r="J24" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="K24" s="69" t="s">
+      <c r="K24" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="L24" s="104" t="s">
+      <c r="L24" s="90" t="s">
         <v>248</v>
       </c>
-      <c r="M24" s="104"/>
-      <c r="N24" s="113" t="s">
+      <c r="M24" s="90"/>
+      <c r="N24" s="91" t="s">
         <v>249</v>
       </c>
-      <c r="O24" s="113"/>
-      <c r="P24" s="112" t="s">
+      <c r="O24" s="91"/>
+      <c r="P24" s="92" t="s">
         <v>250</v>
       </c>
-      <c r="Q24" s="112"/>
-    </row>
-    <row r="25" spans="1:17" ht="22.15" customHeight="1">
-      <c r="A25" s="67">
+      <c r="Q24" s="92"/>
+    </row>
+    <row r="25" spans="1:17" ht="22.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="38">
         <v>11</v>
       </c>
-      <c r="B25" s="108" t="s">
+      <c r="B25" s="89" t="s">
         <v>251</v>
       </c>
-      <c r="C25" s="108"/>
-      <c r="D25" s="108"/>
-      <c r="E25" s="108"/>
-      <c r="F25" s="108"/>
-      <c r="G25" s="108"/>
-      <c r="H25" s="108"/>
-      <c r="I25" s="108"/>
-      <c r="J25" s="68" t="s">
+      <c r="C25" s="89"/>
+      <c r="D25" s="89"/>
+      <c r="E25" s="89"/>
+      <c r="F25" s="89"/>
+      <c r="G25" s="89"/>
+      <c r="H25" s="89"/>
+      <c r="I25" s="89"/>
+      <c r="J25" s="39" t="s">
         <v>252</v>
       </c>
-      <c r="K25" s="69" t="s">
+      <c r="K25" s="40" t="s">
         <v>253</v>
       </c>
-      <c r="L25" s="114" t="s">
+      <c r="L25" s="93" t="s">
         <v>254</v>
       </c>
-      <c r="M25" s="114"/>
-      <c r="N25" s="114"/>
-      <c r="O25" s="114"/>
-      <c r="P25" s="114"/>
-      <c r="Q25" s="114"/>
-    </row>
-    <row r="26" spans="1:17" ht="30" customHeight="1">
-      <c r="A26" s="70">
+      <c r="M25" s="93"/>
+      <c r="N25" s="93"/>
+      <c r="O25" s="93"/>
+      <c r="P25" s="93"/>
+      <c r="Q25" s="93"/>
+    </row>
+    <row r="26" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="41">
         <v>12</v>
       </c>
-      <c r="B26" s="115" t="s">
+      <c r="B26" s="94" t="s">
         <v>255</v>
       </c>
-      <c r="C26" s="115"/>
-      <c r="D26" s="115"/>
-      <c r="E26" s="115"/>
-      <c r="F26" s="115"/>
-      <c r="G26" s="115"/>
-      <c r="H26" s="115"/>
-      <c r="I26" s="115"/>
-      <c r="J26" s="72" t="s">
+      <c r="C26" s="94"/>
+      <c r="D26" s="94"/>
+      <c r="E26" s="94"/>
+      <c r="F26" s="94"/>
+      <c r="G26" s="94"/>
+      <c r="H26" s="94"/>
+      <c r="I26" s="94"/>
+      <c r="J26" s="43" t="s">
         <v>256</v>
       </c>
-      <c r="K26" s="73" t="s">
+      <c r="K26" s="44" t="s">
         <v>257</v>
       </c>
-      <c r="L26" s="71" t="s">
+      <c r="L26" s="42" t="s">
         <v>258</v>
       </c>
-      <c r="M26" s="71" t="s">
+      <c r="M26" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="N26" s="74" t="s">
+      <c r="N26" s="45" t="s">
         <v>210</v>
       </c>
-      <c r="O26" s="74" t="s">
+      <c r="O26" s="45" t="s">
         <v>260</v>
       </c>
-      <c r="P26" s="74" t="s">
+      <c r="P26" s="45" t="s">
         <v>259</v>
       </c>
-      <c r="Q26" s="75" t="s">
+      <c r="Q26" s="46" t="s">
         <v>261</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="106">
-    <mergeCell ref="B24:I24"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="B25:I25"/>
-    <mergeCell ref="L25:Q25"/>
-    <mergeCell ref="B26:I26"/>
-    <mergeCell ref="B21:I21"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="B22:I22"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="B23:I23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="B18:I18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="L19:Q19"/>
-    <mergeCell ref="B20:I20"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="B15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="B16:I16"/>
-    <mergeCell ref="J16:Q16"/>
-    <mergeCell ref="B17:I17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="I1:Q1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="I2:Q4"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:M6"/>
+    <mergeCell ref="N5:O6"/>
+    <mergeCell ref="P5:Q6"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="E6:H6"/>
     <mergeCell ref="A7:A14"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="E7:G7"/>
@@ -5104,26 +5077,68 @@
     <mergeCell ref="P10:Q10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="E11:G11"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L5:M6"/>
-    <mergeCell ref="N5:O6"/>
-    <mergeCell ref="P5:Q6"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="I1:Q1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="I2:Q4"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="B16:I16"/>
+    <mergeCell ref="J16:Q16"/>
+    <mergeCell ref="B17:I17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="B18:I18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="L19:Q19"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="B24:I24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="B25:I25"/>
+    <mergeCell ref="L25:Q25"/>
+    <mergeCell ref="B26:I26"/>
+    <mergeCell ref="B21:I21"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="B22:I22"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="B23:I23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="P23:Q23"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.25" top="0.5" bottom="0.25" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>